<commit_message>
replaced X_SMR_CCS with X_ATR_CCS in the filter file for the conversion script
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kh\Documents\Work\GENeSYS-MOD\Data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D73DF71-597B-49CE-B15D-C4AF66519826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -566,9 +566,6 @@
     <t>X_SMR</t>
   </si>
   <si>
-    <t>X_SMR_CCS</t>
-  </si>
-  <si>
     <t>Z_ETS_Buy</t>
   </si>
   <si>
@@ -894,6 +891,9 @@
   </si>
   <si>
     <t>RES_PV_Utility_Tracking</t>
+  </si>
+  <si>
+    <t>X_ATR_CCS</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -1270,7 +1270,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1576,7 +1576,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1584,7 +1584,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1592,7 +1592,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1600,7 +1600,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1608,7 +1608,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1616,7 +1616,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1624,7 +1624,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1640,7 +1640,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1656,7 +1656,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1664,7 +1664,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1672,7 +1672,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1704,7 +1704,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1719,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,10 +1730,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2666,7 +2666,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2746,15 +2746,15 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>281</v>
+      </c>
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
         <v>162</v>
-      </c>
-      <c r="B128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>163</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2762,15 +2762,15 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="B130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>165</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -2778,15 +2778,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>165</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>166</v>
-      </c>
-      <c r="B132">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2794,15 +2794,15 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
         <v>168</v>
-      </c>
-      <c r="B134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>169</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2810,7 +2810,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2818,7 +2818,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2834,7 +2834,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2842,7 +2842,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -2850,7 +2850,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2858,7 +2858,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2866,7 +2866,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2874,7 +2874,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2898,7 +2898,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2906,7 +2906,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2914,7 +2914,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A137 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A138 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -2934,15 +2934,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2950,7 +2950,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2958,7 +2958,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2974,7 +2974,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2982,7 +2982,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2990,7 +2990,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2998,7 +2998,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3021,15 +3021,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3037,7 +3037,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3045,7 +3045,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3053,7 +3053,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3061,7 +3061,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3069,7 +3069,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3093,7 +3093,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3117,7 +3117,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3125,7 +3125,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3133,7 +3133,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3157,7 +3157,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3181,7 +3181,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3189,7 +3189,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3197,7 +3197,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3205,7 +3205,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3213,7 +3213,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3229,7 +3229,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3237,7 +3237,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3245,7 +3245,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3253,7 +3253,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3261,7 +3261,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3292,10 +3292,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3347,15 +3347,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3378,15 +3378,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3394,7 +3394,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3402,7 +3402,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3410,7 +3410,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3418,7 +3418,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3426,7 +3426,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3434,7 +3434,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3450,7 +3450,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3458,7 +3458,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3466,7 +3466,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3474,7 +3474,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3482,7 +3482,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3490,7 +3490,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3506,7 +3506,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3514,7 +3514,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3522,7 +3522,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3545,15 +3545,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3561,7 +3561,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3569,7 +3569,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3577,7 +3577,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3585,7 +3585,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3609,7 +3609,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3632,7 +3632,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
adding cooling demand and supply
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoeb\Documents\GENeSYS_MOD.data\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4365F530-BD33-4EAA-BEC7-3BF6BA8FADCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="283">
   <si>
     <t>DE</t>
   </si>
@@ -894,6 +894,9 @@
   </si>
   <si>
     <t>X_ATR_CCS</t>
+  </si>
+  <si>
+    <t>Cool_Low_Building</t>
   </si>
 </sst>
 </file>
@@ -961,9 +964,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1001,7 +1004,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1107,7 +1110,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1249,7 +1252,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1719,7 +1722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A109" workbookViewId="0">
       <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
@@ -3011,10 +3014,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3264,6 +3267,14 @@
         <v>213</v>
       </c>
       <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>282</v>
+      </c>
+      <c r="B32">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first try to implement new storage cost data reformulation
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kl\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8FC054-D89E-4D47-A908-492FBC256BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="281">
   <si>
     <t>DE</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>D_PHS</t>
-  </si>
-  <si>
-    <t>D_PHS_Residual</t>
   </si>
   <si>
     <t>FRT_Rail_Conv</t>
@@ -961,9 +958,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1001,7 +998,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1107,7 +1104,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1249,7 +1246,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1270,7 +1267,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1279,7 +1276,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1568,7 +1565,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1576,7 +1573,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1584,7 +1581,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1592,7 +1589,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1600,7 +1597,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1608,7 +1605,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1616,7 +1613,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1624,7 +1621,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1632,7 +1629,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1640,7 +1637,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1648,7 +1645,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1656,7 +1653,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1664,7 +1661,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1672,7 +1669,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1680,7 +1677,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1688,7 +1685,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1696,7 +1693,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1704,7 +1701,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1717,10 +1714,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B148"/>
+  <dimension ref="A1:B147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,10 +1727,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1929,7 +1926,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B26">
@@ -2017,7 +2014,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" t="s">
         <v>72</v>
       </c>
       <c r="B37">
@@ -2433,7 +2430,7 @@
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="2" t="s">
         <v>124</v>
       </c>
       <c r="B89">
@@ -2513,7 +2510,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+      <c r="A99" t="s">
         <v>134</v>
       </c>
       <c r="B99">
@@ -2658,7 +2655,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>152</v>
+        <v>279</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -2666,7 +2663,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>280</v>
+        <v>152</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2738,7 +2735,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>161</v>
+        <v>280</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2746,14 +2743,14 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>281</v>
+        <v>161</v>
       </c>
       <c r="B128">
         <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" s="2" t="s">
         <v>162</v>
       </c>
       <c r="B129">
@@ -2769,7 +2766,7 @@
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
+      <c r="A131" t="s">
         <v>164</v>
       </c>
       <c r="B131">
@@ -2785,7 +2782,7 @@
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" s="2" t="s">
         <v>166</v>
       </c>
       <c r="B133">
@@ -2801,7 +2798,7 @@
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
+      <c r="A135" t="s">
         <v>168</v>
       </c>
       <c r="B135">
@@ -2849,7 +2846,7 @@
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="A141" s="2" t="s">
         <v>174</v>
       </c>
       <c r="B141">
@@ -2857,7 +2854,7 @@
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+      <c r="A142" t="s">
         <v>175</v>
       </c>
       <c r="B142">
@@ -2882,7 +2879,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>178</v>
+        <v>276</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2904,17 +2901,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>279</v>
-      </c>
-      <c r="B148">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A138 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A61 A29:A32 A137 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -2934,15 +2923,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2950,7 +2939,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2958,7 +2947,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2966,7 +2955,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2974,7 +2963,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2982,7 +2971,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2990,7 +2979,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2998,7 +2987,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3021,15 +3010,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3037,7 +3026,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3045,7 +3034,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3053,7 +3042,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3061,7 +3050,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3069,7 +3058,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3077,7 +3066,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3085,7 +3074,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3093,7 +3082,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3101,7 +3090,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3109,7 +3098,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3117,7 +3106,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3125,7 +3114,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3133,7 +3122,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3141,7 +3130,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3149,7 +3138,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3157,7 +3146,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3165,7 +3154,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3173,7 +3162,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3181,7 +3170,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3189,7 +3178,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3197,7 +3186,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3205,7 +3194,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3213,7 +3202,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3221,7 +3210,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3229,7 +3218,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3237,7 +3226,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3245,7 +3234,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3253,7 +3242,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3261,7 +3250,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3292,10 +3281,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>215</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3347,15 +3336,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3378,15 +3367,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3394,7 +3383,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3402,7 +3391,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3410,7 +3399,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3418,7 +3407,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3426,7 +3415,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3434,7 +3423,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3442,7 +3431,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3450,7 +3439,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3458,7 +3447,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3466,7 +3455,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3474,7 +3463,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3482,7 +3471,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3490,7 +3479,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3498,7 +3487,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3506,7 +3495,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3514,7 +3503,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3522,7 +3511,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3545,15 +3534,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3561,7 +3550,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3569,7 +3558,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3577,7 +3566,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3585,7 +3574,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3593,7 +3582,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3601,7 +3590,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3609,7 +3598,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3632,7 +3621,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
Added missing Cool_Low_Building to Sets_Fuel and Set_filter_file
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintef-my.sharepoint.com/personal/morten_svendgard_sintef_no/Documents/Dokumenter/GENeSYS_MOD.data/Conversion Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D16A434-626B-458F-A3B1-07C92A4144B1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="297">
   <si>
     <t>DE</t>
   </si>
@@ -894,6 +894,51 @@
   </si>
   <si>
     <t>X_ATR_CCS</t>
+  </si>
+  <si>
+    <t>HLDH_Biomass_Boiler</t>
+  </si>
+  <si>
+    <t>HLDH_Biomass_CHP</t>
+  </si>
+  <si>
+    <t>HLDH_Coal_Boiler</t>
+  </si>
+  <si>
+    <t>HLDH_Coal_CHP</t>
+  </si>
+  <si>
+    <t>HLDH_Oil_Boiler</t>
+  </si>
+  <si>
+    <t>HLDH_Gas_Boiler</t>
+  </si>
+  <si>
+    <t>HLDH_Gas_CHP</t>
+  </si>
+  <si>
+    <t>HLDH_Geothermal</t>
+  </si>
+  <si>
+    <t>HLDH_Solar_Thermal</t>
+  </si>
+  <si>
+    <t>HLDH_WasteToEnergy_Boiler</t>
+  </si>
+  <si>
+    <t>HLDH_WasteToEnergy_CHP</t>
+  </si>
+  <si>
+    <t>HLDH_Heatpump</t>
+  </si>
+  <si>
+    <t>HLDH_ExcessHeat</t>
+  </si>
+  <si>
+    <t>HLDH_Electric_Boiler</t>
+  </si>
+  <si>
+    <t>Cool_Low_Building</t>
   </si>
 </sst>
 </file>
@@ -960,10 +1005,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1001,7 +1050,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1107,7 +1156,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1249,7 +1298,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1259,11 +1308,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -1717,13 +1766,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B148"/>
+  <dimension ref="A1:B162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
@@ -2912,6 +2961,118 @@
         <v>1</v>
       </c>
     </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>282</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>283</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>284</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>285</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>286</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>287</v>
+      </c>
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>288</v>
+      </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>289</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>290</v>
+      </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>291</v>
+      </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>292</v>
+      </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>293</v>
+      </c>
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>294</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>295</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A138 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
@@ -2919,6 +3080,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2930,7 +3092,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3011,13 +3173,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3173,7 +3338,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>296</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3181,7 +3346,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3189,7 +3354,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3197,7 +3362,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3205,7 +3370,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3213,7 +3378,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3221,7 +3386,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3229,7 +3394,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3237,7 +3402,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3245,7 +3410,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3253,7 +3418,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3261,18 +3426,26 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>213</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A29:A30" xr:uid="{B8609C0C-A954-452A-ACA7-8E39C5A6D865}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A30:A31" xr:uid="{B8609C0C-A954-452A-ACA7-8E39C5A6D865}">
       <formula1>Fuels</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A26" xr:uid="{D2F2E49F-8FE0-4740-B1E5-B2C92E5D2E8B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27" xr:uid="{D2F2E49F-8FE0-4740-B1E5-B2C92E5D2E8B}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -3288,7 +3461,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3343,7 +3516,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3374,7 +3547,7 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3541,7 +3714,7 @@
       <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3625,10 +3798,10 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Adding tech, fuel, and storage to filter
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintef-my.sharepoint.com/personal/morten_svendgard_sintef_no/Documents/Dokumenter/GENeSYS_MOD.data/Conversion Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D16A434-626B-458F-A3B1-07C92A4144B1}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3506CFB-CCF1-450B-9198-90DFB7FFB07F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="304">
   <si>
     <t>DE</t>
   </si>
@@ -939,6 +939,27 @@
   </si>
   <si>
     <t>Cool_Low_Building</t>
+  </si>
+  <si>
+    <t>Heat_Low_DistrictHeat</t>
+  </si>
+  <si>
+    <t>S_Heat_HLB</t>
+  </si>
+  <si>
+    <t>S_Heat_HLDH</t>
+  </si>
+  <si>
+    <t>HLDH_Heatpump_Air</t>
+  </si>
+  <si>
+    <t>HLDH_Heatpump_ExcessHeat</t>
+  </si>
+  <si>
+    <t>HLI_Heatpump</t>
+  </si>
+  <si>
+    <t>HMLI_Heatpump</t>
   </si>
 </sst>
 </file>
@@ -1766,10 +1787,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B162"/>
+  <dimension ref="A1:B166"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A161" sqref="A161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3070,6 +3091,38 @@
         <v>295</v>
       </c>
       <c r="B162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>300</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>301</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>302</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>303</v>
+      </c>
+      <c r="B166">
         <v>1</v>
       </c>
     </row>
@@ -3086,13 +3139,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82051EE-CB34-4773-B6E9-985CB3357CE5}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3163,6 +3220,22 @@
         <v>225</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>299</v>
+      </c>
+      <c r="B11">
         <v>1</v>
       </c>
     </row>
@@ -3173,15 +3246,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3346,7 +3419,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>203</v>
+        <v>297</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3354,7 +3427,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3362,7 +3435,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3370,7 +3443,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3378,7 +3451,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3386,7 +3459,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3394,7 +3467,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3402,7 +3475,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3410,7 +3483,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3418,7 +3491,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3426,7 +3499,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3434,18 +3507,26 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>212</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>213</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A30:A31" xr:uid="{B8609C0C-A954-452A-ACA7-8E39C5A6D865}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A31:A32" xr:uid="{B8609C0C-A954-452A-ACA7-8E39C5A6D865}">
       <formula1>Fuels</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A27" xr:uid="{D2F2E49F-8FE0-4740-B1E5-B2C92E5D2E8B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A28" xr:uid="{D2F2E49F-8FE0-4740-B1E5-B2C92E5D2E8B}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added Heat_Low_DistrictHeat where missing, D_Heat_HLR where missing, removed techs with missing data, so on ...
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sintef-my.sharepoint.com/personal/morten_svendgard_sintef_no/Documents/Dokumenter/GENeSYS_MOD.data/Conversion Script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3506CFB-CCF1-450B-9198-90DFB7FFB07F}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD946010-7E07-4F9A-9FA3-2B52F1BE30D0}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -905,18 +905,12 @@
     <t>HLDH_Coal_Boiler</t>
   </si>
   <si>
-    <t>HLDH_Coal_CHP</t>
-  </si>
-  <si>
     <t>HLDH_Oil_Boiler</t>
   </si>
   <si>
     <t>HLDH_Gas_Boiler</t>
   </si>
   <si>
-    <t>HLDH_Gas_CHP</t>
-  </si>
-  <si>
     <t>HLDH_Geothermal</t>
   </si>
   <si>
@@ -960,6 +954,12 @@
   </si>
   <si>
     <t>HMLI_Heatpump</t>
+  </si>
+  <si>
+    <t>Waste</t>
+  </si>
+  <si>
+    <t>Heat_Low_Building</t>
   </si>
 </sst>
 </file>
@@ -1333,12 +1333,12 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>254</v>
       </c>
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>258</v>
       </c>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1404,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1444,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1500,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1532,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>259</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>260</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>261</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>262</v>
       </c>
@@ -1668,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>263</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>264</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>265</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>266</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>267</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>268</v>
       </c>
@@ -1716,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>269</v>
       </c>
@@ -1724,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>270</v>
       </c>
@@ -1732,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>271</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>272</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>273</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>274</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>275</v>
       </c>
@@ -1772,7 +1772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>276</v>
       </c>
@@ -1787,18 +1787,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B166"/>
+  <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A161" sqref="A161"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="E156" sqref="E156"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>181</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1814,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1838,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1862,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1894,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1902,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1934,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1982,7 +1982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>62</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>63</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>64</v>
       </c>
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>65</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>66</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>67</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>68</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>69</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
@@ -2078,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>71</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>73</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>75</v>
       </c>
@@ -2118,7 +2118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>76</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>77</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>78</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>81</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>83</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>84</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>85</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -2206,7 +2206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>87</v>
       </c>
@@ -2214,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>88</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>89</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>90</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>91</v>
       </c>
@@ -2246,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>92</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>93</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>94</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>95</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>96</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>97</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>98</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>99</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>100</v>
       </c>
@@ -2318,7 +2318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>103</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>104</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>105</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>106</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>107</v>
       </c>
@@ -2374,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>108</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>109</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>110</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>111</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>112</v>
       </c>
@@ -2414,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>113</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>114</v>
       </c>
@@ -2430,7 +2430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>115</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>116</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>117</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>118</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>119</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>120</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>121</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>122</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>123</v>
       </c>
@@ -2502,7 +2502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>124</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>125</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>126</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>127</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>128</v>
       </c>
@@ -2542,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>129</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="2" t="s">
         <v>130</v>
       </c>
@@ -2558,7 +2558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>131</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>132</v>
       </c>
@@ -2574,7 +2574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>133</v>
       </c>
@@ -2582,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>134</v>
       </c>
@@ -2590,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>135</v>
       </c>
@@ -2598,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>136</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>137</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>138</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>139</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>140</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>141</v>
       </c>
@@ -2646,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>142</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>143</v>
       </c>
@@ -2662,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>144</v>
       </c>
@@ -2670,7 +2670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>145</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>146</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>147</v>
       </c>
@@ -2694,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>148</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>149</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>150</v>
       </c>
@@ -2718,7 +2718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>151</v>
       </c>
@@ -2726,7 +2726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>152</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>280</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>153</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>154</v>
       </c>
@@ -2758,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>155</v>
       </c>
@@ -2766,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>156</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>157</v>
       </c>
@@ -2782,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>158</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>159</v>
       </c>
@@ -2798,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>160</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>161</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>281</v>
       </c>
@@ -2822,7 +2822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>162</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="2" t="s">
         <v>163</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>164</v>
       </c>
@@ -2846,7 +2846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>165</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>166</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>167</v>
       </c>
@@ -2870,7 +2870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>168</v>
       </c>
@@ -2878,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>169</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>170</v>
       </c>
@@ -2894,7 +2894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>171</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>172</v>
       </c>
@@ -2910,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>173</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>174</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>175</v>
       </c>
@@ -2934,7 +2934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>176</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>177</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>178</v>
       </c>
@@ -2958,7 +2958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>277</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>278</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>279</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>282</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>283</v>
       </c>
@@ -2998,7 +2998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>284</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>285</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>286</v>
       </c>
@@ -3022,7 +3022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>287</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>288</v>
       </c>
@@ -3038,7 +3038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>289</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>290</v>
       </c>
@@ -3054,23 +3054,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>291</v>
       </c>
       <c r="B158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>292</v>
       </c>
       <c r="B159">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>293</v>
       </c>
@@ -3078,23 +3078,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="B161">
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="B162">
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>300</v>
       </c>
@@ -3102,27 +3102,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>301</v>
       </c>
       <c r="B164">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>302</v>
-      </c>
-      <c r="B165">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>303</v>
-      </c>
-      <c r="B166">
         <v>1</v>
       </c>
     </row>
@@ -3145,13 +3129,13 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>217</v>
       </c>
@@ -3159,7 +3143,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>218</v>
       </c>
@@ -3167,7 +3151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>219</v>
       </c>
@@ -3175,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>220</v>
       </c>
@@ -3183,7 +3167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -3191,7 +3175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -3199,7 +3183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>223</v>
       </c>
@@ -3207,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>224</v>
       </c>
@@ -3215,7 +3199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>225</v>
       </c>
@@ -3223,17 +3207,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3246,18 +3230,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>184</v>
       </c>
@@ -3265,7 +3249,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -3273,7 +3257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>186</v>
       </c>
@@ -3281,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>187</v>
       </c>
@@ -3289,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>188</v>
       </c>
@@ -3297,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>189</v>
       </c>
@@ -3305,7 +3289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>190</v>
       </c>
@@ -3313,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>191</v>
       </c>
@@ -3321,7 +3305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>192</v>
       </c>
@@ -3329,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>193</v>
       </c>
@@ -3337,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>194</v>
       </c>
@@ -3345,7 +3329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>195</v>
       </c>
@@ -3353,7 +3337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>196</v>
       </c>
@@ -3361,7 +3345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>197</v>
       </c>
@@ -3369,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>198</v>
       </c>
@@ -3377,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>199</v>
       </c>
@@ -3385,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>200</v>
       </c>
@@ -3393,7 +3377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>201</v>
       </c>
@@ -3401,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>202</v>
       </c>
@@ -3409,124 +3393,140 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>203</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
         <v>204</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
         <v>205</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>206</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>207</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>208</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>209</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>204</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
         <v>210</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
         <v>211</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
         <v>212</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
         <v>213</v>
       </c>
-      <c r="B33">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>302</v>
+      </c>
+      <c r="B35">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A31:A32" xr:uid="{B8609C0C-A954-452A-ACA7-8E39C5A6D865}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A32:A33" xr:uid="{B8609C0C-A954-452A-ACA7-8E39C5A6D865}">
       <formula1>Fuels</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A28" xr:uid="{D2F2E49F-8FE0-4740-B1E5-B2C92E5D2E8B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A29" xr:uid="{D2F2E49F-8FE0-4740-B1E5-B2C92E5D2E8B}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -3542,9 +3542,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>215</v>
       </c>
@@ -3552,7 +3552,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3597,9 +3597,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>179</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -3628,9 +3628,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>257</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>227</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>228</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>229</v>
       </c>
@@ -3662,7 +3662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>230</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>231</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>232</v>
       </c>
@@ -3686,7 +3686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>233</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>234</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>235</v>
       </c>
@@ -3710,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>236</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>237</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>238</v>
       </c>
@@ -3734,7 +3734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>239</v>
       </c>
@@ -3742,7 +3742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>240</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>241</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>242</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>243</v>
       </c>
@@ -3774,7 +3774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>244</v>
       </c>
@@ -3795,9 +3795,9 @@
       <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>256</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>193</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>246</v>
       </c>
@@ -3821,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>247</v>
       </c>
@@ -3829,7 +3829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>248</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>249</v>
       </c>
@@ -3845,7 +3845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>250</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>251</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>252</v>
       </c>
@@ -3882,9 +3882,9 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>255</v>
       </c>
@@ -3893,7 +3893,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -3909,7 +3909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2030</v>
       </c>
@@ -3941,7 +3941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2035</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2040</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2045</v>
       </c>
@@ -3965,7 +3965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2050</v>
       </c>

</xml_diff>

<commit_message>
Rename technologies: HLR_ -> HB_ (Heat Building and CB for Cooling Building later on); RES_ -> P_ (for RES technologies that generate electricity); RES_ -> R_ (for Biomass technologies, since they are resources); Added rename script;
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EA695D-29A3-4AB2-AC88-B731B69EE8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B765F9-8DAF-4D6B-8298-6E9AB6750DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="38280" yWindow="15" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Year_selection" sheetId="4" r:id="rId9"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$148</definedName>
     <definedName name="Fuels">#REF!</definedName>
     <definedName name="Technologies">#REF!:B</definedName>
   </definedNames>
@@ -272,9 +273,6 @@
     <t>HLI_Convert_DH</t>
   </si>
   <si>
-    <t>HLR_Convert_DH</t>
-  </si>
-  <si>
     <t>HHI_BF_BOF</t>
   </si>
   <si>
@@ -329,39 +327,6 @@
     <t>HLI_Solar_Thermal</t>
   </si>
   <si>
-    <t>HLR_Biomass</t>
-  </si>
-  <si>
-    <t>HLR_Direct_Electric</t>
-  </si>
-  <si>
-    <t>HLR_Gas_Boiler</t>
-  </si>
-  <si>
-    <t>HLR_Geothermal</t>
-  </si>
-  <si>
-    <t>HLR_H2_Boiler</t>
-  </si>
-  <si>
-    <t>HLR_Hardcoal</t>
-  </si>
-  <si>
-    <t>HLR_Heatpump_Aerial</t>
-  </si>
-  <si>
-    <t>HLR_Heatpump_Ground</t>
-  </si>
-  <si>
-    <t>HLR_Lignite</t>
-  </si>
-  <si>
-    <t>HLR_Oil_Boiler</t>
-  </si>
-  <si>
-    <t>HLR_Solar_Thermal</t>
-  </si>
-  <si>
     <t>HMI_Biomass</t>
   </si>
   <si>
@@ -470,72 +435,6 @@
     <t>R_Oil</t>
   </si>
   <si>
-    <t>RES_Biogas</t>
-  </si>
-  <si>
-    <t>RES_CSP</t>
-  </si>
-  <si>
-    <t>RES_Geothermal</t>
-  </si>
-  <si>
-    <t>RES_Grass</t>
-  </si>
-  <si>
-    <t>RES_Hydro_Large</t>
-  </si>
-  <si>
-    <t>RES_Hydro_Small</t>
-  </si>
-  <si>
-    <t>RES_Ocean</t>
-  </si>
-  <si>
-    <t>RES_Paper_Cardboard</t>
-  </si>
-  <si>
-    <t>RES_PV_Rooftop_Commercial</t>
-  </si>
-  <si>
-    <t>RES_PV_Rooftop_Residential</t>
-  </si>
-  <si>
-    <t>RES_PV_Utility_Avg</t>
-  </si>
-  <si>
-    <t>RES_PV_Utility_Inf</t>
-  </si>
-  <si>
-    <t>RES_PV_Utility_Opt</t>
-  </si>
-  <si>
-    <t>RES_Residues</t>
-  </si>
-  <si>
-    <t>RES_Roundwood</t>
-  </si>
-  <si>
-    <t>RES_Wind_Offshore_Deep</t>
-  </si>
-  <si>
-    <t>RES_Wind_Offshore_Shallow</t>
-  </si>
-  <si>
-    <t>RES_Wind_Offshore_Transitional</t>
-  </si>
-  <si>
-    <t>RES_Wind_Onshore_Avg</t>
-  </si>
-  <si>
-    <t>RES_Wind_Onshore_Inf</t>
-  </si>
-  <si>
-    <t>RES_Wind_Onshore_Opt</t>
-  </si>
-  <si>
-    <t>RES_Wood</t>
-  </si>
-  <si>
     <t>X_Biofuel</t>
   </si>
   <si>
@@ -890,10 +789,112 @@
     <t>X_SOEC_Electrolysis</t>
   </si>
   <si>
-    <t>RES_PV_Utility_Tracking</t>
-  </si>
-  <si>
     <t>X_ATR_CCS</t>
+  </si>
+  <si>
+    <t>HB_Biomass</t>
+  </si>
+  <si>
+    <t>HB_Convert_DH</t>
+  </si>
+  <si>
+    <t>HB_Direct_Electric</t>
+  </si>
+  <si>
+    <t>HB_Gas_Boiler</t>
+  </si>
+  <si>
+    <t>HB_Geothermal</t>
+  </si>
+  <si>
+    <t>HB_H2_Boiler</t>
+  </si>
+  <si>
+    <t>HB_Hardcoal</t>
+  </si>
+  <si>
+    <t>HB_Heatpump_Aerial</t>
+  </si>
+  <si>
+    <t>HB_Heatpump_Ground</t>
+  </si>
+  <si>
+    <t>HB_Lignite</t>
+  </si>
+  <si>
+    <t>HB_Oil_Boiler</t>
+  </si>
+  <si>
+    <t>HB_Solar_Thermal</t>
+  </si>
+  <si>
+    <t>R_Biogas</t>
+  </si>
+  <si>
+    <t>R_Grass</t>
+  </si>
+  <si>
+    <t>R_Paper_Cardboard</t>
+  </si>
+  <si>
+    <t>R_Residues</t>
+  </si>
+  <si>
+    <t>R_Roundwood</t>
+  </si>
+  <si>
+    <t>R_Wood</t>
+  </si>
+  <si>
+    <t>P_CSP</t>
+  </si>
+  <si>
+    <t>P_Geothermal</t>
+  </si>
+  <si>
+    <t>P_Hydro_Large</t>
+  </si>
+  <si>
+    <t>P_Hydro_Small</t>
+  </si>
+  <si>
+    <t>P_Ocean</t>
+  </si>
+  <si>
+    <t>P_PV_Rooftop_Commercial</t>
+  </si>
+  <si>
+    <t>P_PV_Rooftop_Residential</t>
+  </si>
+  <si>
+    <t>P_PV_Utility_Avg</t>
+  </si>
+  <si>
+    <t>P_PV_Utility_Inf</t>
+  </si>
+  <si>
+    <t>P_PV_Utility_Opt</t>
+  </si>
+  <si>
+    <t>P_PV_Utility_Tracking</t>
+  </si>
+  <si>
+    <t>P_Wind_Offshore_Deep</t>
+  </si>
+  <si>
+    <t>P_Wind_Offshore_Shallow</t>
+  </si>
+  <si>
+    <t>P_Wind_Offshore_Transitional</t>
+  </si>
+  <si>
+    <t>P_Wind_Onshore_Avg</t>
+  </si>
+  <si>
+    <t>P_Wind_Onshore_Inf</t>
+  </si>
+  <si>
+    <t>P_Wind_Onshore_Opt</t>
   </si>
 </sst>
 </file>
@@ -961,9 +962,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1001,7 +1002,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1107,7 +1108,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1249,7 +1250,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1270,7 +1271,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>254</v>
+        <v>220</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1279,7 +1280,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>258</v>
+        <v>224</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1568,7 +1569,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>225</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1576,7 +1577,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1584,7 +1585,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>261</v>
+        <v>227</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1592,7 +1593,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>262</v>
+        <v>228</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1600,7 +1601,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>263</v>
+        <v>229</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1608,7 +1609,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>264</v>
+        <v>230</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1616,7 +1617,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>231</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1624,7 +1625,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>266</v>
+        <v>232</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1632,7 +1633,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>267</v>
+        <v>233</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1640,7 +1641,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>268</v>
+        <v>234</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1648,7 +1649,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>269</v>
+        <v>235</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1656,7 +1657,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1664,7 +1665,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1672,7 +1673,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>272</v>
+        <v>238</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1680,7 +1681,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>273</v>
+        <v>239</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1688,7 +1689,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1696,7 +1697,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1704,7 +1705,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>276</v>
+        <v>242</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1719,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B129" sqref="B129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,10 +1731,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>183</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2026,7 +2027,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>73</v>
+        <v>247</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2034,7 +2035,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>248</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2042,7 +2043,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>75</v>
+        <v>249</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2050,7 +2051,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>76</v>
+        <v>250</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2058,7 +2059,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>77</v>
+        <v>251</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2066,7 +2067,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>252</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2074,7 +2075,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>253</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2082,7 +2083,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>254</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2090,7 +2091,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>255</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2098,7 +2099,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>256</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2106,7 +2107,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>257</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2114,7 +2115,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>84</v>
+        <v>258</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2122,7 +2123,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2130,7 +2131,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2138,7 +2139,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2146,7 +2147,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2154,7 +2155,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2162,7 +2163,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -2170,7 +2171,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2178,7 +2179,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -2186,7 +2187,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -2194,7 +2195,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2202,7 +2203,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -2210,7 +2211,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2218,7 +2219,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2226,7 +2227,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2234,7 +2235,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2242,7 +2243,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2250,7 +2251,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2258,7 +2259,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2266,7 +2267,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2274,7 +2275,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2282,7 +2283,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2290,7 +2291,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2298,7 +2299,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2306,7 +2307,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2314,7 +2315,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2322,7 +2323,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2330,7 +2331,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2338,7 +2339,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2346,7 +2347,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2354,7 +2355,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2362,7 +2363,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2370,7 +2371,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2378,7 +2379,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -2386,7 +2387,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>118</v>
+        <v>265</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2394,7 +2395,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2402,7 +2403,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2410,7 +2411,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2418,7 +2419,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2426,7 +2427,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>123</v>
+        <v>266</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2434,87 +2435,87 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B89">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>125</v>
+      <c r="A90" t="s">
+        <v>267</v>
       </c>
       <c r="B90">
         <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>126</v>
+      <c r="A91" t="s">
+        <v>268</v>
       </c>
       <c r="B91">
         <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>127</v>
+      <c r="A92" t="s">
+        <v>111</v>
       </c>
       <c r="B92">
         <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>128</v>
+      <c r="A93" t="s">
+        <v>269</v>
       </c>
       <c r="B93">
         <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
-        <v>129</v>
+      <c r="A94" t="s">
+        <v>112</v>
       </c>
       <c r="B94">
         <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
-        <v>130</v>
+      <c r="A95" t="s">
+        <v>270</v>
       </c>
       <c r="B95">
         <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>131</v>
+      <c r="A96" t="s">
+        <v>271</v>
       </c>
       <c r="B96">
         <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
-        <v>132</v>
+      <c r="A97" t="s">
+        <v>272</v>
       </c>
       <c r="B97">
         <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>133</v>
+      <c r="A98" t="s">
+        <v>273</v>
       </c>
       <c r="B98">
         <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
-        <v>134</v>
+      <c r="A99" t="s">
+        <v>274</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2522,7 +2523,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>135</v>
+        <v>275</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2530,7 +2531,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>136</v>
+        <v>276</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2538,7 +2539,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>137</v>
+        <v>277</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2546,7 +2547,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>138</v>
+        <v>278</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2554,7 +2555,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>139</v>
+        <v>279</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2562,7 +2563,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>140</v>
+        <v>280</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2570,87 +2571,87 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>141</v>
+        <v>281</v>
       </c>
       <c r="B106">
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>142</v>
+      <c r="A107" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>143</v>
+      <c r="A108" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="B108">
         <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>144</v>
+      <c r="A109" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="B109">
         <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>145</v>
+      <c r="A110" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="B110">
         <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>146</v>
+      <c r="A111" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B111">
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>147</v>
+      <c r="A112" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="B112">
         <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>148</v>
+      <c r="A113" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="B113">
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>149</v>
+      <c r="A114" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B114">
         <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>150</v>
+      <c r="A115" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="B115">
         <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>151</v>
+      <c r="A116" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -2658,7 +2659,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>152</v>
+        <v>259</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -2666,7 +2667,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>280</v>
+        <v>123</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2674,7 +2675,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -2682,7 +2683,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -2690,7 +2691,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>155</v>
+        <v>260</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -2698,7 +2699,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2706,7 +2707,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2714,7 +2715,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>158</v>
+        <v>261</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -2722,7 +2723,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>159</v>
+        <v>262</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2730,7 +2731,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>160</v>
+        <v>263</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2738,7 +2739,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>161</v>
+        <v>264</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2746,7 +2747,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2754,15 +2755,15 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>162</v>
+        <v>246</v>
       </c>
       <c r="B129">
         <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>163</v>
+      <c r="A130" t="s">
+        <v>128</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -2770,15 +2771,15 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="B131">
         <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>165</v>
+      <c r="A132" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -2786,15 +2787,15 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>167</v>
+      <c r="A134" t="s">
+        <v>132</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -2802,15 +2803,15 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="B135">
         <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>169</v>
+      <c r="A136" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2818,7 +2819,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -2826,7 +2827,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>171</v>
+        <v>244</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2834,7 +2835,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2842,7 +2843,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>173</v>
+        <v>137</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -2850,15 +2851,15 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>174</v>
+        <v>245</v>
       </c>
       <c r="B141">
         <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
-        <v>175</v>
+      <c r="A142" t="s">
+        <v>138</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2866,7 +2867,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>176</v>
+        <v>139</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2874,15 +2875,15 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>177</v>
+        <v>140</v>
       </c>
       <c r="B144">
         <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>178</v>
+      <c r="A145" s="2" t="s">
+        <v>141</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2890,7 +2891,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>277</v>
+        <v>142</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2898,7 +2899,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>278</v>
+        <v>143</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2906,13 +2907,18 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>279</v>
+        <v>144</v>
       </c>
       <c r="B148">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:B148" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B148">
+      <sortCondition ref="A1:A148"/>
+    </sortState>
+  </autoFilter>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A138 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
@@ -2934,15 +2940,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>217</v>
+        <v>183</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>218</v>
+        <v>184</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2950,7 +2956,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>219</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2958,7 +2964,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>220</v>
+        <v>186</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2966,7 +2972,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>221</v>
+        <v>187</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2974,7 +2980,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>222</v>
+        <v>188</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2982,7 +2988,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>223</v>
+        <v>189</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2990,7 +2996,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>190</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -2998,7 +3004,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>191</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3021,15 +3027,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>214</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3037,7 +3043,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3045,7 +3051,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3053,7 +3059,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>154</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3061,7 +3067,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>189</v>
+        <v>155</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3069,7 +3075,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>156</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3077,7 +3083,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3085,7 +3091,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>192</v>
+        <v>158</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3093,7 +3099,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3101,7 +3107,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>194</v>
+        <v>160</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3109,7 +3115,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3117,7 +3123,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3125,7 +3131,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3133,7 +3139,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3141,7 +3147,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3149,7 +3155,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>200</v>
+        <v>166</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3157,7 +3163,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>201</v>
+        <v>167</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3165,7 +3171,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>168</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3173,7 +3179,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>203</v>
+        <v>169</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3181,7 +3187,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3189,7 +3195,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>205</v>
+        <v>171</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3197,7 +3203,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>206</v>
+        <v>172</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3205,7 +3211,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>207</v>
+        <v>173</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3213,7 +3219,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3221,7 +3227,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>209</v>
+        <v>175</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3229,7 +3235,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3237,7 +3243,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>210</v>
+        <v>176</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3245,7 +3251,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>211</v>
+        <v>177</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3253,7 +3259,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>212</v>
+        <v>178</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3261,7 +3267,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3292,10 +3298,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>215</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>216</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3347,15 +3353,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>182</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3378,15 +3384,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>245</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>227</v>
+        <v>193</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3394,7 +3400,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3402,7 +3408,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>229</v>
+        <v>195</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3410,7 +3416,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>196</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3418,7 +3424,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3426,7 +3432,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>232</v>
+        <v>198</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3434,7 +3440,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>233</v>
+        <v>199</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3442,7 +3448,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>234</v>
+        <v>200</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3450,7 +3456,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>235</v>
+        <v>201</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3458,7 +3464,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>202</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3466,7 +3472,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>203</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3474,7 +3480,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>204</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3482,7 +3488,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>205</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3490,7 +3496,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>240</v>
+        <v>206</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3498,7 +3504,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>241</v>
+        <v>207</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3506,7 +3512,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3514,7 +3520,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3522,7 +3528,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3545,15 +3551,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>256</v>
+        <v>222</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>253</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3561,7 +3567,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3569,7 +3575,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3577,7 +3583,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3585,7 +3591,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3593,7 +3599,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>250</v>
+        <v>216</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3601,7 +3607,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>217</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3609,7 +3615,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3632,7 +3638,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>255</v>
+        <v>221</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
renaming: D_Heat_HLR -> D_Heat_HB; S_Heat_HLR -> S_Heat_HB; Heat_Low_Residential -> Heat_Buildings
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B765F9-8DAF-4D6B-8298-6E9AB6750DBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A1DFD5-000E-45F7-A7A8-24768515B3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="15" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -228,9 +228,6 @@
     <t>D_Heat_HLI</t>
   </si>
   <si>
-    <t>D_Heat_HLR</t>
-  </si>
-  <si>
     <t>D_PHS</t>
   </si>
   <si>
@@ -546,9 +543,6 @@
     <t>Gas_Synth</t>
   </si>
   <si>
-    <t>Heat_Low_Residential</t>
-  </si>
-  <si>
     <t>Heat_Low_Industrial</t>
   </si>
   <si>
@@ -615,9 +609,6 @@
     <t>S_Battery_Redox</t>
   </si>
   <si>
-    <t>S_Heat_HLR</t>
-  </si>
-  <si>
     <t>S_Heat_HLI</t>
   </si>
   <si>
@@ -895,6 +886,15 @@
   </si>
   <si>
     <t>P_Wind_Onshore_Opt</t>
+  </si>
+  <si>
+    <t>D_Heat_HB</t>
+  </si>
+  <si>
+    <t>S_Heat_HB</t>
+  </si>
+  <si>
+    <t>Heat_Buildings</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1271,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1280,7 +1280,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1569,7 +1569,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1577,7 +1577,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1585,7 +1585,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1593,7 +1593,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1601,7 +1601,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1609,7 +1609,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1617,7 +1617,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1625,7 +1625,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1641,7 +1641,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1649,7 +1649,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1657,7 +1657,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1665,7 +1665,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1673,7 +1673,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1681,7 +1681,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1720,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,10 +1731,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1915,7 +1915,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>279</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1923,7 +1923,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1931,7 +1931,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1947,7 +1947,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1955,7 +1955,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1987,7 +1987,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1995,7 +1995,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2003,7 +2003,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -2019,7 +2019,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -2027,7 +2027,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2035,7 +2035,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2043,7 +2043,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2059,7 +2059,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2075,7 +2075,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2139,7 +2139,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2147,7 +2147,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2155,7 +2155,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2163,7 +2163,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -2171,7 +2171,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2179,7 +2179,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -2187,7 +2187,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -2195,7 +2195,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2203,7 +2203,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2219,7 +2219,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2227,7 +2227,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2235,7 +2235,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2243,7 +2243,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2267,7 +2267,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2291,7 +2291,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2299,7 +2299,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2307,7 +2307,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2315,7 +2315,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2331,7 +2331,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2339,7 +2339,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2355,7 +2355,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2371,7 +2371,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2379,7 +2379,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -2387,7 +2387,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2395,7 +2395,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2403,7 +2403,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2411,7 +2411,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2419,7 +2419,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2443,7 +2443,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2459,7 +2459,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2499,7 +2499,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2515,7 +2515,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2555,7 +2555,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2571,7 +2571,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -2579,7 +2579,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -2595,7 +2595,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -2603,7 +2603,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -2611,7 +2611,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -2619,7 +2619,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B113">
         <v>1</v>
@@ -2635,7 +2635,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -2643,7 +2643,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -2659,7 +2659,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2675,7 +2675,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -2699,7 +2699,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2707,7 +2707,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2715,7 +2715,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -2723,7 +2723,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2731,7 +2731,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2747,7 +2747,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2763,7 +2763,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -2771,7 +2771,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -2779,7 +2779,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -2787,7 +2787,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -2803,7 +2803,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2811,7 +2811,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2819,7 +2819,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2835,7 +2835,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2843,7 +2843,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -2851,7 +2851,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2859,7 +2859,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2867,7 +2867,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -2883,7 +2883,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2899,7 +2899,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2907,7 +2907,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2933,22 +2933,25 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2956,7 +2959,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2964,7 +2967,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2972,7 +2975,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2980,7 +2983,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>188</v>
+        <v>280</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2988,7 +2991,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -2996,7 +2999,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3004,7 +3007,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3019,23 +3022,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3043,7 +3049,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3051,7 +3057,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3059,7 +3065,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3067,7 +3073,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3075,7 +3081,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3083,7 +3089,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3091,7 +3097,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3099,7 +3105,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3107,7 +3113,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3115,7 +3121,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3123,7 +3129,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3131,7 +3137,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3139,7 +3145,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3147,7 +3153,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>165</v>
+        <v>281</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3155,7 +3161,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3163,7 +3169,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3171,7 +3177,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3179,7 +3185,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3187,7 +3193,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3195,7 +3201,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3203,7 +3209,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3211,7 +3217,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3219,7 +3225,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3227,7 +3233,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3235,7 +3241,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3243,7 +3249,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3251,7 +3257,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3259,7 +3265,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3267,7 +3273,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3298,10 +3304,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3353,15 +3359,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3384,15 +3390,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3400,7 +3406,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3408,7 +3414,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3416,7 +3422,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3424,7 +3430,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3432,7 +3438,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3440,7 +3446,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3448,7 +3454,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3456,7 +3462,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3464,7 +3470,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3472,7 +3478,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3480,7 +3486,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3488,7 +3494,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3496,7 +3502,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3504,7 +3510,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3512,7 +3518,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3520,7 +3526,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3528,7 +3534,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3551,15 +3557,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3567,7 +3573,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3575,7 +3581,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3583,7 +3589,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3591,7 +3597,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3599,7 +3605,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3607,7 +3613,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3615,7 +3621,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3638,7 +3644,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
deleted empty line in AnnualExogenousEmission; updated hydro technology names in filter file
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72A1DFD5-000E-45F7-A7A8-24768515B3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E54952-63F6-448C-BC8A-6573727563BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -843,12 +843,6 @@
     <t>P_Geothermal</t>
   </si>
   <si>
-    <t>P_Hydro_Large</t>
-  </si>
-  <si>
-    <t>P_Hydro_Small</t>
-  </si>
-  <si>
     <t>P_Ocean</t>
   </si>
   <si>
@@ -895,6 +889,12 @@
   </si>
   <si>
     <t>Heat_Buildings</t>
+  </si>
+  <si>
+    <t>P_Hydro_Reservoir</t>
+  </si>
+  <si>
+    <t>P_Hydro_RoR</t>
   </si>
 </sst>
 </file>
@@ -1720,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,7 +1915,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2443,7 +2443,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>264</v>
+        <v>280</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2451,7 +2451,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2467,7 +2467,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2483,7 +2483,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2499,7 +2499,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2507,7 +2507,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2515,7 +2515,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2523,7 +2523,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2539,7 +2539,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2555,7 +2555,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2563,7 +2563,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2571,7 +2571,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3022,7 +3022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -3153,7 +3153,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B16">
         <v>1</v>

</xml_diff>

<commit_message>
added H2_Blend to ensure that runs work properly, since it is hard coded in the equations
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E54952-63F6-448C-BC8A-6573727563BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C41E65A-DF02-4577-AFA1-43A86970C3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="283">
   <si>
     <t>DE</t>
   </si>
@@ -895,6 +895,9 @@
   </si>
   <si>
     <t>P_Hydro_RoR</t>
+  </si>
+  <si>
+    <t>H2_Blend</t>
   </si>
 </sst>
 </file>
@@ -1720,7 +1723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A92" sqref="A92"/>
     </sheetView>
   </sheetViews>
@@ -3020,10 +3023,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3041,7 +3044,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3049,7 +3052,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3057,7 +3060,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3065,7 +3068,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3073,7 +3076,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3081,7 +3084,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3089,7 +3092,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>175</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3097,7 +3100,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>176</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3105,7 +3108,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3113,7 +3116,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3121,7 +3124,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3129,7 +3132,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3137,7 +3140,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>282</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3145,7 +3148,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3161,7 +3164,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3169,7 +3172,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3177,7 +3180,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3185,7 +3188,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3193,7 +3196,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3201,7 +3204,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3209,7 +3212,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3217,7 +3220,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3225,7 +3228,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3233,7 +3236,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3241,7 +3244,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3249,7 +3252,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3257,7 +3260,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3265,7 +3268,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3273,13 +3276,24 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
     </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
+    <sortCondition ref="A1:A32"/>
+  </sortState>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A29:A30" xr:uid="{B8609C0C-A954-452A-ACA7-8E39C5A6D865}">
       <formula1>Fuels</formula1>

</xml_diff>

<commit_message>
updated filter file to match new technology names
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C41E65A-DF02-4577-AFA1-43A86970C3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321883E9-F4BB-4B89-8998-B33381B9D4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Year_selection" sheetId="4" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$149</definedName>
     <definedName name="Fuels">#REF!</definedName>
     <definedName name="Technologies">#REF!:B</definedName>
   </definedNames>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="284">
   <si>
     <t>DE</t>
   </si>
@@ -324,30 +324,6 @@
     <t>HLI_Solar_Thermal</t>
   </si>
   <si>
-    <t>HMI_Biomass</t>
-  </si>
-  <si>
-    <t>HMI_H2</t>
-  </si>
-  <si>
-    <t>HMI_Gas</t>
-  </si>
-  <si>
-    <t>HMI_Gas_CCS</t>
-  </si>
-  <si>
-    <t>HMI_HardCoal</t>
-  </si>
-  <si>
-    <t>HMI_HardCoal_CCS</t>
-  </si>
-  <si>
-    <t>HMI_Oil</t>
-  </si>
-  <si>
-    <t>HMI_Steam_Electric</t>
-  </si>
-  <si>
     <t>P_Biomass</t>
   </si>
   <si>
@@ -898,6 +874,33 @@
   </si>
   <si>
     <t>H2_Blend</t>
+  </si>
+  <si>
+    <t>HMHI_Biomass</t>
+  </si>
+  <si>
+    <t>HMHI_Gas</t>
+  </si>
+  <si>
+    <t>HMHI_Gas_CCS</t>
+  </si>
+  <si>
+    <t>HMHI_H2</t>
+  </si>
+  <si>
+    <t>HMHI_HardCoal</t>
+  </si>
+  <si>
+    <t>HMHI_HardCoal_CCS</t>
+  </si>
+  <si>
+    <t>HMHI_Oil</t>
+  </si>
+  <si>
+    <t>HMHI_Steam_Electric</t>
+  </si>
+  <si>
+    <t>HMLI_Heatpump</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1277,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1283,7 +1286,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1572,7 +1575,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1580,7 +1583,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1588,7 +1591,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1596,7 +1599,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1604,7 +1607,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1612,7 +1615,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1620,7 +1623,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1628,7 +1631,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1636,7 +1639,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1644,7 +1647,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1652,7 +1655,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1660,7 +1663,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1668,7 +1671,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1676,7 +1679,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1684,7 +1687,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1692,7 +1695,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1700,7 +1703,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1708,7 +1711,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1721,10 +1724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B148"/>
+  <dimension ref="A1:B149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="Q72" sqref="Q72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,10 +1737,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1918,7 +1921,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2030,7 +2033,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2038,7 +2041,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2046,7 +2049,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2054,7 +2057,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2062,7 +2065,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2070,7 +2073,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2078,7 +2081,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2086,7 +2089,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2094,7 +2097,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2102,7 +2105,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2110,7 +2113,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2118,7 +2121,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2278,7 +2281,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>91</v>
+        <v>275</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2286,7 +2289,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>276</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2294,7 +2297,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>94</v>
+        <v>277</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2302,7 +2305,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>92</v>
+        <v>278</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2310,7 +2313,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>95</v>
+        <v>279</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2318,7 +2321,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>96</v>
+        <v>280</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2326,7 +2329,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>97</v>
+        <v>281</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2334,7 +2337,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>98</v>
+        <v>282</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2342,7 +2345,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>99</v>
+        <v>283</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2350,7 +2353,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2358,7 +2361,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2366,7 +2369,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2374,7 +2377,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2382,7 +2385,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -2390,7 +2393,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>262</v>
+        <v>96</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2398,7 +2401,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>105</v>
+        <v>254</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2406,7 +2409,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2414,7 +2417,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2422,7 +2425,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2430,7 +2433,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>263</v>
+        <v>99</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2438,7 +2441,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>109</v>
+        <v>255</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2446,7 +2449,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>280</v>
+        <v>101</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2454,7 +2457,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2462,7 +2465,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>110</v>
+        <v>273</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2470,7 +2473,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>264</v>
+        <v>102</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2478,7 +2481,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>111</v>
+        <v>256</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2486,7 +2489,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>265</v>
+        <v>103</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2494,7 +2497,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2502,7 +2505,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2510,7 +2513,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2518,7 +2521,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2526,7 +2529,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2534,7 +2537,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2542,7 +2545,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2550,7 +2553,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2558,7 +2561,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2566,7 +2569,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2574,15 +2577,15 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B106">
         <v>1</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>112</v>
+      <c r="A107" t="s">
+        <v>268</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2590,7 +2593,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -2598,7 +2601,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -2606,7 +2609,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -2614,7 +2617,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -2622,7 +2625,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2630,7 +2633,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B113">
         <v>1</v>
@@ -2638,7 +2641,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -2646,7 +2649,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -2654,15 +2657,15 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B116">
         <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>256</v>
+      <c r="A117" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -2670,7 +2673,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>122</v>
+        <v>248</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2678,7 +2681,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -2686,7 +2689,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -2694,7 +2697,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>257</v>
+        <v>116</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -2702,7 +2705,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>125</v>
+        <v>249</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2710,7 +2713,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2718,7 +2721,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>258</v>
+        <v>118</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -2726,7 +2729,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2734,7 +2737,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2742,7 +2745,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2750,7 +2753,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2758,7 +2761,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2766,15 +2769,15 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>235</v>
       </c>
       <c r="B130">
         <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>128</v>
+      <c r="A131" t="s">
+        <v>119</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -2782,15 +2785,15 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B132">
         <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>130</v>
+      <c r="A133" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2798,15 +2801,15 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B134">
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>132</v>
+      <c r="A135" t="s">
+        <v>123</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2814,15 +2817,15 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B136">
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>134</v>
+      <c r="A137" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -2830,7 +2833,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>241</v>
+        <v>126</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2838,7 +2841,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>135</v>
+        <v>233</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2846,7 +2849,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -2854,7 +2857,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>242</v>
+        <v>128</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2862,7 +2865,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>137</v>
+        <v>234</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2870,7 +2873,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2878,23 +2881,23 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="B144">
         <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>140</v>
+      <c r="A145" t="s">
+        <v>131</v>
       </c>
       <c r="B145">
         <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>141</v>
+      <c r="A146" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2902,7 +2905,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2910,20 +2913,28 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B148">
         <v>1</v>
       </c>
     </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>135</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B148" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B148">
-      <sortCondition ref="A1:A148"/>
+  <autoFilter ref="A1:B149" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B149">
+      <sortCondition ref="A1:A149"/>
     </sortState>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A138 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A139 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -2946,15 +2957,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2962,7 +2973,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2970,7 +2981,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2978,7 +2989,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2986,7 +2997,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2994,7 +3005,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3002,7 +3013,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3010,7 +3021,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3025,7 +3036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -3036,15 +3047,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3052,7 +3063,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3060,7 +3071,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3068,7 +3079,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3076,7 +3087,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3084,7 +3095,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3092,7 +3103,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3100,7 +3111,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3108,7 +3119,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3116,7 +3127,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3124,7 +3135,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3132,7 +3143,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3140,7 +3151,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3148,7 +3159,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3156,7 +3167,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3164,7 +3175,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3172,7 +3183,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3180,7 +3191,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3188,7 +3199,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3196,7 +3207,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3204,7 +3215,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3212,7 +3223,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3220,7 +3231,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3228,7 +3239,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3236,7 +3247,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3244,7 +3255,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3252,7 +3263,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3260,7 +3271,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3268,7 +3279,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3276,7 +3287,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3284,7 +3295,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3318,10 +3329,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3373,15 +3384,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3404,15 +3415,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3420,7 +3431,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3428,7 +3439,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3436,7 +3447,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3444,7 +3455,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3452,7 +3463,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3460,7 +3471,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3468,7 +3479,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3476,7 +3487,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3484,7 +3495,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3492,7 +3503,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3500,7 +3511,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3508,7 +3519,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3516,7 +3527,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3524,7 +3535,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3532,7 +3543,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3540,7 +3551,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3548,7 +3559,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3571,15 +3582,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3587,7 +3598,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3595,7 +3606,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3603,7 +3614,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3611,7 +3622,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3619,7 +3630,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3627,7 +3638,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3635,7 +3646,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3658,7 +3669,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
removed X_Fuel_Cell as it is obsolete
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321883E9-F4BB-4B89-8998-B33381B9D4E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE06AAAA-8914-42A4-B27A-37868E28E02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
@@ -24,7 +24,7 @@
     <sheet name="Year_selection" sheetId="4" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$148</definedName>
     <definedName name="Fuels">#REF!</definedName>
     <definedName name="Technologies">#REF!:B</definedName>
   </definedNames>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="283">
   <si>
     <t>DE</t>
   </si>
@@ -415,9 +415,6 @@
   </si>
   <si>
     <t>X_DAC_LT</t>
-  </si>
-  <si>
-    <t>X_Electrolysis</t>
   </si>
   <si>
     <t>X_Fuel_Cell</t>
@@ -1277,7 +1274,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1286,7 +1283,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1575,7 +1572,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1583,7 +1580,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1591,7 +1588,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1599,7 +1596,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1607,7 +1604,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1615,7 +1612,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1623,7 +1620,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1631,7 +1628,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1639,7 +1636,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1647,7 +1644,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1655,7 +1652,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1663,7 +1660,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1671,7 +1668,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1679,7 +1676,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1687,7 +1684,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1695,7 +1692,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1703,7 +1700,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1711,7 +1708,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1724,10 +1721,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B149"/>
+  <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="Q72" sqref="Q72"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="E134" sqref="E134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,10 +1734,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1921,7 +1918,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2033,7 +2030,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2041,7 +2038,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2049,7 +2046,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2057,7 +2054,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2065,7 +2062,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2073,7 +2070,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2081,7 +2078,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2089,7 +2086,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2097,7 +2094,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2105,7 +2102,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2113,7 +2110,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2121,7 +2118,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2281,7 +2278,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2289,7 +2286,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2297,7 +2294,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2305,7 +2302,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2313,7 +2310,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2321,7 +2318,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2329,7 +2326,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2337,7 +2334,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2345,7 +2342,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2401,7 +2398,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2441,7 +2438,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2457,7 +2454,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2465,7 +2462,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2481,7 +2478,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2497,7 +2494,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2505,7 +2502,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2513,7 +2510,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2521,7 +2518,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2529,7 +2526,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2537,7 +2534,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2545,7 +2542,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2553,7 +2550,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2561,7 +2558,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2569,7 +2566,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2577,7 +2574,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -2585,7 +2582,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2673,7 +2670,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2705,7 +2702,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2729,7 +2726,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2737,7 +2734,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2745,7 +2742,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2753,7 +2750,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2761,7 +2758,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2769,7 +2766,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -2808,7 +2805,7 @@
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B135">
@@ -2824,7 +2821,7 @@
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
+      <c r="A137" t="s">
         <v>125</v>
       </c>
       <c r="B137">
@@ -2833,7 +2830,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>126</v>
+        <v>232</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2841,7 +2838,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>233</v>
+        <v>126</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2857,7 +2854,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>128</v>
+        <v>233</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2865,7 +2862,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>234</v>
+        <v>128</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2888,7 +2885,7 @@
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="A145" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B145">
@@ -2896,7 +2893,7 @@
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
+      <c r="A146" t="s">
         <v>132</v>
       </c>
       <c r="B146">
@@ -2919,22 +2916,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>135</v>
-      </c>
-      <c r="B149">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B149" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B149">
-      <sortCondition ref="A1:A149"/>
+  <autoFilter ref="A1:B148" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B148">
+      <sortCondition ref="A1:A148"/>
     </sortState>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A139 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A138 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -2957,15 +2946,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2973,7 +2962,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2981,7 +2970,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2989,7 +2978,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2997,7 +2986,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3005,7 +2994,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3013,7 +3002,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3021,7 +3010,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3047,15 +3036,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3063,7 +3052,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3071,7 +3060,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3079,7 +3068,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3087,7 +3076,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3095,7 +3084,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3103,7 +3092,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3111,7 +3100,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3119,7 +3108,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3127,7 +3116,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3135,7 +3124,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3143,7 +3132,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3151,7 +3140,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3159,7 +3148,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3167,7 +3156,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3175,7 +3164,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3183,7 +3172,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3191,7 +3180,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3199,7 +3188,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3207,7 +3196,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3215,7 +3204,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3223,7 +3212,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3231,7 +3220,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3239,7 +3228,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3247,7 +3236,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3255,7 +3244,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3263,7 +3252,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3271,7 +3260,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3279,7 +3268,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3287,7 +3276,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3295,7 +3284,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3329,10 +3318,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3384,15 +3373,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3415,15 +3404,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3431,7 +3420,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3439,7 +3428,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3447,7 +3436,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3455,7 +3444,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3463,7 +3452,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3471,7 +3460,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3479,7 +3468,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3487,7 +3476,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3495,7 +3484,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3503,7 +3492,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3511,7 +3500,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3519,7 +3508,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3527,7 +3516,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3535,7 +3524,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3543,7 +3532,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3551,7 +3540,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3559,7 +3548,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3582,15 +3571,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3598,7 +3587,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3606,7 +3595,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3614,7 +3603,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3622,7 +3611,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3630,7 +3619,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3638,7 +3627,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3646,7 +3635,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3669,7 +3658,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
fixed mistake in previous commit, now actually removed X_Fuel_Cell
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE06AAAA-8914-42A4-B27A-37868E28E02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108F7C9D-9DA9-4150-A312-0B050210746B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
@@ -417,9 +417,6 @@
     <t>X_DAC_LT</t>
   </si>
   <si>
-    <t>X_Fuel_Cell</t>
-  </si>
-  <si>
     <t>X_Gasifier</t>
   </si>
   <si>
@@ -898,6 +895,9 @@
   </si>
   <si>
     <t>HMLI_Heatpump</t>
+  </si>
+  <si>
+    <t>X_Electrolysis</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1274,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1283,7 +1283,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1580,7 +1580,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1588,7 +1588,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1596,7 +1596,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1604,7 +1604,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1612,7 +1612,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1620,7 +1620,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1628,7 +1628,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1636,7 +1636,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1668,7 +1668,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1676,7 +1676,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1684,7 +1684,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1700,7 +1700,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1724,7 +1724,7 @@
   <dimension ref="A1:B148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="E134" sqref="E134"/>
+      <selection activeCell="F133" sqref="F133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,10 +1734,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1918,7 +1918,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -2030,7 +2030,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2038,7 +2038,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2046,7 +2046,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2054,7 +2054,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2062,7 +2062,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2070,7 +2070,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2078,7 +2078,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2086,7 +2086,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2094,7 +2094,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2110,7 +2110,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2278,7 +2278,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2286,7 +2286,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2294,7 +2294,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2310,7 +2310,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2318,7 +2318,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2326,7 +2326,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2334,7 +2334,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2342,7 +2342,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2398,7 +2398,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2438,7 +2438,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2454,7 +2454,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2478,7 +2478,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2494,7 +2494,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2502,7 +2502,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2510,7 +2510,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2518,7 +2518,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2526,7 +2526,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2534,7 +2534,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2542,7 +2542,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2558,7 +2558,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2574,7 +2574,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2702,7 +2702,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2726,7 +2726,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2742,7 +2742,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2750,7 +2750,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2766,7 +2766,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -2798,7 +2798,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>122</v>
+        <v>282</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -2806,7 +2806,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2822,7 +2822,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -2830,7 +2830,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2838,7 +2838,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2846,7 +2846,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -2854,7 +2854,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2870,7 +2870,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2894,7 +2894,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2910,7 +2910,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2946,15 +2946,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2962,7 +2962,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2970,7 +2970,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2986,7 +2986,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3010,7 +3010,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3036,15 +3036,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3052,7 +3052,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3060,7 +3060,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3076,7 +3076,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3100,7 +3100,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3108,7 +3108,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3116,7 +3116,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3124,7 +3124,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3132,7 +3132,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3140,7 +3140,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3148,7 +3148,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3172,7 +3172,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3180,7 +3180,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3188,7 +3188,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3212,7 +3212,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3220,7 +3220,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3244,7 +3244,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3252,7 +3252,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3260,7 +3260,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3268,7 +3268,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3276,7 +3276,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3284,7 +3284,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3318,10 +3318,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3373,15 +3373,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3404,15 +3404,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3428,7 +3428,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3436,7 +3436,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3444,7 +3444,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3452,7 +3452,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3460,7 +3460,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3468,7 +3468,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3476,7 +3476,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3484,7 +3484,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3492,7 +3492,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3500,7 +3500,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3508,7 +3508,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3516,7 +3516,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3524,7 +3524,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3540,7 +3540,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3571,15 +3571,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3587,7 +3587,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3595,7 +3595,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3603,7 +3603,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3611,7 +3611,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3619,7 +3619,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3627,7 +3627,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3635,7 +3635,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3658,7 +3658,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
fixed bug in availabilityfactor data
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{108F7C9D-9DA9-4150-A312-0B050210746B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E226ACA-A21E-4CF6-9FC5-2929886FB8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
@@ -1723,8 +1723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F133" sqref="F133"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1937,7 @@
         <v>60</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added new heat storages from commit bc9e25ccb353a6e9da0ec50b37c00254dfa64255 to Set_filter_file.xlsx
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E226ACA-A21E-4CF6-9FC5-2929886FB8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFE0FE2-2A18-413F-9155-F56B57CE3451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,8 @@
     <sheet name="Year_selection" sheetId="4" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$148</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Storage_selection!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$149</definedName>
     <definedName name="Fuels">#REF!</definedName>
     <definedName name="Technologies">#REF!:B</definedName>
   </definedNames>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="285">
   <si>
     <t>DE</t>
   </si>
@@ -225,9 +226,6 @@
     <t>D_Gas_Methane</t>
   </si>
   <si>
-    <t>D_Heat_HLI</t>
-  </si>
-  <si>
     <t>D_PHS</t>
   </si>
   <si>
@@ -579,9 +577,6 @@
     <t>S_Battery_Redox</t>
   </si>
   <si>
-    <t>S_Heat_HLI</t>
-  </si>
-  <si>
     <t>S_CAES</t>
   </si>
   <si>
@@ -852,12 +847,6 @@
     <t>P_Wind_Onshore_Opt</t>
   </si>
   <si>
-    <t>D_Heat_HB</t>
-  </si>
-  <si>
-    <t>S_Heat_HB</t>
-  </si>
-  <si>
     <t>Heat_Buildings</t>
   </si>
   <si>
@@ -898,6 +887,24 @@
   </si>
   <si>
     <t>X_Electrolysis</t>
+  </si>
+  <si>
+    <t>D_HLI_Tank_Large</t>
+  </si>
+  <si>
+    <t>D_HB_Tank_Small</t>
+  </si>
+  <si>
+    <t>D_HD_Pit</t>
+  </si>
+  <si>
+    <t>S_HB_Tank_Small</t>
+  </si>
+  <si>
+    <t>S_HLI_Tank_Large</t>
+  </si>
+  <si>
+    <t>S_HD_Pit</t>
   </si>
 </sst>
 </file>
@@ -1274,7 +1281,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1283,7 +1290,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1572,7 +1579,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1580,7 +1587,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1588,7 +1595,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1596,7 +1603,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1604,7 +1611,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1612,7 +1619,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1620,7 +1627,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1628,7 +1635,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1636,7 +1643,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1644,7 +1651,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1652,7 +1659,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1660,7 +1667,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1668,7 +1675,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1676,7 +1683,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1684,7 +1691,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1692,7 +1699,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1700,7 +1707,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1708,7 +1715,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1721,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B148"/>
+  <dimension ref="A1:B149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1734,10 +1741,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1910,7 +1917,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>279</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -1918,7 +1925,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1926,7 +1933,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>281</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1934,23 +1941,23 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27">
         <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27">
-        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1958,7 +1965,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1966,7 +1973,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1974,7 +1981,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1982,7 +1989,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1990,7 +1997,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1998,7 +2005,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2006,7 +2013,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -2014,7 +2021,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -2022,15 +2029,15 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>234</v>
+      <c r="A38" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -2038,7 +2045,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2046,7 +2053,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2054,7 +2061,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2062,7 +2069,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2070,7 +2077,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2078,7 +2085,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2086,7 +2093,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2094,7 +2101,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2102,7 +2109,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2110,7 +2117,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2118,7 +2125,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2126,7 +2133,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>243</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2134,7 +2141,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2142,7 +2149,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2150,7 +2157,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2158,7 +2165,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2166,7 +2173,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -2174,7 +2181,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2182,7 +2189,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -2190,7 +2197,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -2198,7 +2205,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2206,7 +2213,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -2214,7 +2221,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2222,7 +2229,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2230,7 +2237,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2238,7 +2245,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2246,7 +2253,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2254,7 +2261,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2262,7 +2269,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2270,7 +2277,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2278,7 +2285,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>273</v>
+        <v>89</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2286,7 +2293,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2294,7 +2301,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2302,7 +2309,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2310,7 +2317,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2318,7 +2325,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2326,7 +2333,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2334,7 +2341,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2342,7 +2349,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2350,7 +2357,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>91</v>
+        <v>277</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2358,7 +2365,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2366,7 +2373,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2374,7 +2381,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2382,7 +2389,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -2390,7 +2397,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2398,7 +2405,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>252</v>
+        <v>95</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2406,7 +2413,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>97</v>
+        <v>250</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2414,7 +2421,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2422,7 +2429,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2430,7 +2437,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2438,7 +2445,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>253</v>
+        <v>98</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2446,7 +2453,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>101</v>
+        <v>251</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2454,7 +2461,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>270</v>
+        <v>100</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2462,7 +2469,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2470,7 +2477,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>267</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2478,7 +2485,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>254</v>
+        <v>101</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2486,7 +2493,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>103</v>
+        <v>252</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2494,7 +2501,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>255</v>
+        <v>102</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2502,7 +2509,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2510,7 +2517,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2518,7 +2525,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2526,7 +2533,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2534,7 +2541,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2542,7 +2549,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2550,7 +2557,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2558,7 +2565,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2566,7 +2573,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2574,7 +2581,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -2582,15 +2589,15 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B107">
         <v>1</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>104</v>
+      <c r="A108" t="s">
+        <v>264</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -2598,7 +2605,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -2606,7 +2613,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -2614,7 +2621,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -2622,7 +2629,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2630,7 +2637,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B113">
         <v>1</v>
@@ -2638,7 +2645,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -2646,7 +2653,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -2654,7 +2661,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -2662,15 +2669,15 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B117">
         <v>1</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>246</v>
+      <c r="A118" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2678,7 +2685,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>114</v>
+        <v>244</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -2686,7 +2693,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -2694,7 +2701,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -2702,7 +2709,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>247</v>
+        <v>115</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2710,7 +2717,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>117</v>
+        <v>245</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2718,7 +2725,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -2726,7 +2733,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>248</v>
+        <v>117</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2734,7 +2741,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2742,7 +2749,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2750,7 +2757,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2758,7 +2765,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>230</v>
+        <v>249</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2766,7 +2773,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -2774,15 +2781,15 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>119</v>
+        <v>231</v>
       </c>
       <c r="B131">
         <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>120</v>
+      <c r="A132" t="s">
+        <v>118</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -2790,23 +2797,23 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>282</v>
+      <c r="A134" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B134">
         <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>122</v>
+      <c r="A135" t="s">
+        <v>278</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2814,15 +2821,15 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B136">
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>124</v>
+      <c r="A137" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -2830,7 +2837,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>231</v>
+        <v>123</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2838,7 +2845,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>125</v>
+        <v>229</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2846,7 +2853,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B140">
         <v>1</v>
@@ -2854,7 +2861,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>232</v>
+        <v>125</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2862,7 +2869,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>127</v>
+        <v>230</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2870,7 +2877,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2878,23 +2885,23 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
+        <v>127</v>
+      </c>
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>128</v>
+      </c>
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>131</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2902,7 +2909,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2910,20 +2917,28 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B148">
         <v>1</v>
       </c>
     </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>132</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:B148" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B148">
-      <sortCondition ref="A1:A148"/>
+  <autoFilter ref="A1:B149" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B149">
+      <sortCondition ref="A1:A149"/>
     </sortState>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A62 A30:A33 A138 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A63 A31:A34 A139 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -2933,10 +2948,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82051EE-CB34-4773-B6E9-985CB3357CE5}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2946,15 +2961,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2962,7 +2977,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2970,7 +2985,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2978,7 +2993,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -2986,7 +3001,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>176</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2994,7 +3009,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>176</v>
+        <v>282</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3002,7 +3017,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>177</v>
+        <v>284</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3010,13 +3025,26 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>178</v>
+        <v>283</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>171</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:B1" xr:uid="{B82051EE-CB34-4773-B6E9-985CB3357CE5}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3036,15 +3064,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3052,7 +3080,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3060,7 +3088,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3068,7 +3096,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3076,7 +3104,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3084,7 +3112,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3092,7 +3120,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3100,7 +3128,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3108,7 +3136,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3116,7 +3144,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3124,7 +3152,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3132,7 +3160,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3140,7 +3168,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3148,7 +3176,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3156,7 +3184,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3164,7 +3192,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3172,7 +3200,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3180,7 +3208,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3188,7 +3216,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3196,7 +3224,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3204,7 +3232,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3212,7 +3240,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3220,7 +3248,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3228,7 +3256,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3236,7 +3264,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3244,7 +3272,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3252,7 +3280,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3260,7 +3288,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3268,7 +3296,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3276,7 +3304,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3284,7 +3312,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3318,10 +3346,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -3373,15 +3401,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3404,15 +3432,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3420,7 +3448,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3428,7 +3456,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3436,7 +3464,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3444,7 +3472,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3452,7 +3480,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3460,7 +3488,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3468,7 +3496,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3476,7 +3504,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3484,7 +3512,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3492,7 +3520,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3500,7 +3528,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3508,7 +3536,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3516,7 +3544,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3524,7 +3552,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3532,7 +3560,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3540,7 +3568,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3548,7 +3576,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3571,15 +3599,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3587,7 +3615,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3595,7 +3623,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3603,7 +3631,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3611,7 +3639,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3619,7 +3647,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3627,7 +3655,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3635,7 +3663,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3658,7 +3686,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
added missing HD technologies to filter file
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFE0FE2-2A18-413F-9155-F56B57CE3451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997A6E23-96CE-434C-A514-9E37F295C482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Storage_selection!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$154</definedName>
     <definedName name="Fuels">#REF!</definedName>
     <definedName name="Technologies">#REF!:B</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="290">
   <si>
     <t>DE</t>
   </si>
@@ -905,6 +905,21 @@
   </si>
   <si>
     <t>S_HD_Pit</t>
+  </si>
+  <si>
+    <t>HD_Electric_Boiler</t>
+  </si>
+  <si>
+    <t>HD_Geothermal</t>
+  </si>
+  <si>
+    <t>HD_Heatpump_Air</t>
+  </si>
+  <si>
+    <t>HD_Heatpump_ExcessHeat</t>
+  </si>
+  <si>
+    <t>HD_Solar_Thermal</t>
   </si>
 </sst>
 </file>
@@ -1728,10 +1743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B149"/>
+  <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2141,7 +2156,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>72</v>
+        <v>285</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2149,7 +2164,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>286</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2157,7 +2172,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>287</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2165,7 +2180,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>288</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2173,7 +2188,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>289</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -2181,7 +2196,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2189,7 +2204,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -2197,7 +2212,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -2205,7 +2220,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2213,7 +2228,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -2221,7 +2236,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2229,7 +2244,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -2237,7 +2252,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2245,7 +2260,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2253,7 +2268,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2261,7 +2276,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2269,7 +2284,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2277,7 +2292,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2285,7 +2300,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2293,7 +2308,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>269</v>
+        <v>85</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2301,7 +2316,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>270</v>
+        <v>86</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2309,7 +2324,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>271</v>
+        <v>87</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2317,7 +2332,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>272</v>
+        <v>88</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2325,7 +2340,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>273</v>
+        <v>89</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2333,7 +2348,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2341,7 +2356,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2349,7 +2364,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -2357,7 +2372,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2365,7 +2380,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>273</v>
       </c>
       <c r="B79">
         <v>1</v>
@@ -2373,7 +2388,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>274</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2381,7 +2396,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>92</v>
+        <v>275</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -2389,7 +2404,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>276</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -2397,7 +2412,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>277</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2405,7 +2420,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2413,7 +2428,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>250</v>
+        <v>91</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2421,7 +2436,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2429,7 +2444,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2437,7 +2452,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2445,7 +2460,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2453,7 +2468,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2461,7 +2476,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2469,7 +2484,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>266</v>
+        <v>99</v>
       </c>
       <c r="B92">
         <v>1</v>
@@ -2477,7 +2492,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>267</v>
+        <v>97</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2485,7 +2500,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2493,7 +2508,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2501,7 +2516,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2509,7 +2524,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>253</v>
+        <v>266</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2517,7 +2532,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>254</v>
+        <v>267</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2525,7 +2540,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>255</v>
+        <v>101</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2533,7 +2548,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2541,7 +2556,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>257</v>
+        <v>102</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2549,7 +2564,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2557,7 +2572,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2565,7 +2580,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -2573,7 +2588,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B105">
         <v>1</v>
@@ -2581,7 +2596,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B106">
         <v>1</v>
@@ -2589,7 +2604,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B107">
         <v>1</v>
@@ -2597,47 +2612,47 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
+        <v>259</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>260</v>
+      </c>
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>261</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>262</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>263</v>
+      </c>
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
         <v>264</v>
-      </c>
-      <c r="B108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="B111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="B113">
         <v>1</v>
@@ -2645,7 +2660,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -2653,7 +2668,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -2661,7 +2676,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -2669,7 +2684,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -2677,47 +2692,47 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>244</v>
-      </c>
-      <c r="B119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>113</v>
-      </c>
-      <c r="B120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>114</v>
-      </c>
-      <c r="B121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>115</v>
-      </c>
-      <c r="B122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>245</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2725,7 +2740,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>116</v>
+        <v>244</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -2733,7 +2748,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2741,7 +2756,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>246</v>
+        <v>114</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2749,7 +2764,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>247</v>
+        <v>115</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2757,7 +2772,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -2765,7 +2780,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>249</v>
+        <v>116</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2773,7 +2788,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>228</v>
+        <v>117</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -2781,7 +2796,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -2789,23 +2804,23 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>118</v>
+        <v>247</v>
       </c>
       <c r="B132">
         <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>119</v>
+      <c r="A133" t="s">
+        <v>248</v>
       </c>
       <c r="B133">
         <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>120</v>
+      <c r="A134" t="s">
+        <v>249</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -2813,39 +2828,39 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>278</v>
+        <v>228</v>
       </c>
       <c r="B135">
         <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>121</v>
+      <c r="A136" t="s">
+        <v>231</v>
       </c>
       <c r="B136">
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>122</v>
+      <c r="A137" t="s">
+        <v>118</v>
       </c>
       <c r="B137">
         <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>123</v>
+      <c r="A138" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="B138">
         <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>229</v>
+      <c r="A139" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2853,23 +2868,23 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>124</v>
+        <v>278</v>
       </c>
       <c r="B140">
         <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>125</v>
+      <c r="A141" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="B141">
         <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>230</v>
+      <c r="A142" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2877,7 +2892,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2885,7 +2900,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>127</v>
+        <v>229</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -2893,15 +2908,15 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B145">
         <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
-        <v>129</v>
+      <c r="A146" t="s">
+        <v>125</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2909,7 +2924,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>130</v>
+        <v>230</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2917,7 +2932,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2925,20 +2940,60 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
+        <v>127</v>
+      </c>
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>128</v>
+      </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>130</v>
+      </c>
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>131</v>
+      </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
         <v>132</v>
       </c>
-      <c r="B149">
+      <c r="B154">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B149" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B149">
-      <sortCondition ref="A1:A149"/>
+  <autoFilter ref="A1:B154" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B154">
+      <sortCondition ref="A1:A154"/>
     </sortState>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A63 A31:A34 A139 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A68 A31:A34 A144 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -2950,7 +3005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82051EE-CB34-4773-B6E9-985CB3357CE5}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed issues with TagTechnologyToSubsets and TagFuelToSubsets adding compatibility for both new Heat Medium High/Low and old Heat Medium formulations
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997A6E23-96CE-434C-A514-9E37F295C482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74330DBF-4971-47E3-A8DD-E350BD1F79D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="292">
   <si>
     <t>DE</t>
   </si>
@@ -920,6 +920,12 @@
   </si>
   <si>
     <t>HD_Solar_Thermal</t>
+  </si>
+  <si>
+    <t>Heat_MediumLow_Industrial</t>
+  </si>
+  <si>
+    <t>Heat_MediumHigh_Industrial</t>
   </si>
 </sst>
 </file>
@@ -1745,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3106,15 +3112,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3274,12 +3280,12 @@
         <v>154</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>159</v>
+        <v>290</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3287,7 +3293,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>161</v>
+        <v>291</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3295,7 +3301,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3303,7 +3309,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3311,7 +3317,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3319,7 +3325,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3327,7 +3333,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3335,7 +3341,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3343,7 +3349,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3351,7 +3357,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3359,7 +3365,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3367,21 +3373,37 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>147</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>157</v>
       </c>
-      <c r="B32">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B32">
-    <sortCondition ref="A1:A32"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B34">
+    <sortCondition ref="A1:A34"/>
   </sortState>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A29:A30" xr:uid="{B8609C0C-A954-452A-ACA7-8E39C5A6D865}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A14 A31:A32" xr:uid="{B8609C0C-A954-452A-ACA7-8E39C5A6D865}">
       <formula1>Fuels</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A26" xr:uid="{D2F2E49F-8FE0-4740-B1E5-B2C92E5D2E8B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A28" xr:uid="{D2F2E49F-8FE0-4740-B1E5-B2C92E5D2E8B}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added 2018 cost data; Added some more Technologies to Subsets
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74330DBF-4971-47E3-A8DD-E350BD1F79D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4EEEDC-DCDB-496F-851A-10965EF0A38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -1291,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,8 +1751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,7 +3114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -3413,10 +3413,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A951553-3765-459F-BC61-BDBD26E96FE5}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3458,6 +3458,22 @@
         <v>4</v>
       </c>
       <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
     </row>
@@ -3755,7 +3771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D817F8-1014-4E28-A827-54661E8BA006}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added 2055 and 2060 (for now same as 2050)
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4EEEDC-DCDB-496F-851A-10965EF0A38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D32C5DD-7956-420D-B265-322E6D2439FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -3769,10 +3769,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D817F8-1014-4E28-A827-54661E8BA006}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3820,15 +3820,15 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2025</v>
+        <v>2021</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2030</v>
+        <v>2025</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3836,7 +3836,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3844,7 +3844,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2040</v>
+        <v>2035</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3852,7 +3852,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3860,9 +3860,33 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>2045</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>2050</v>
       </c>
-      <c r="B11">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2055</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2060</v>
+      </c>
+      <c r="B14">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 2021 as base year by using interpolation between 2018 and 2025. Works except for "ModalSplit" and transport demand
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D32C5DD-7956-420D-B265-322E6D2439FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D764D80-482C-4394-8543-41B5DC3D3AFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
@@ -3772,7 +3772,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3799,7 +3799,7 @@
         <v>2018</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3823,7 +3823,7 @@
         <v>2021</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
some fixes for debugging in conversion script; removed utf-8 error in timeseries
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\test_lotr\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D32C5DD-7956-420D-B265-322E6D2439FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5358071F-C144-4EF0-BF51-BFF2EDCB99D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="297">
   <si>
     <t>DE</t>
   </si>
@@ -926,6 +926,21 @@
   </si>
   <si>
     <t>Heat_MediumHigh_Industrial</t>
+  </si>
+  <si>
+    <t>DolAmroth</t>
+  </si>
+  <si>
+    <t>Gondor</t>
+  </si>
+  <si>
+    <t>Rohan</t>
+  </si>
+  <si>
+    <t>Harad</t>
+  </si>
+  <si>
+    <t>Mordor</t>
   </si>
 </sst>
 </file>
@@ -1289,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1378,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1371,7 +1386,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1379,7 +1394,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1387,7 +1402,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1395,7 +1410,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1403,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1411,7 +1426,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1419,7 +1434,7 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1427,7 +1442,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1435,7 +1450,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1443,7 +1458,7 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1451,7 +1466,7 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1459,7 +1474,7 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1467,7 +1482,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1475,7 +1490,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1483,7 +1498,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1491,7 +1506,7 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,7 +1514,7 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1507,7 +1522,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1515,7 +1530,7 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1523,7 +1538,7 @@
         <v>1</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1531,7 +1546,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1539,7 +1554,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1547,7 +1562,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1555,7 +1570,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1563,7 +1578,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,7 +1586,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1579,7 +1594,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1587,7 +1602,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1595,7 +1610,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1740,6 +1755,46 @@
       </c>
       <c r="B55">
         <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>292</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>293</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>294</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>295</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>296</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3771,7 +3826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D817F8-1014-4E28-A827-54661E8BA006}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated set_filter file to include newest technologies recalibrated residualcapacities slightly to work with all time resolutions
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\testbed\Documents\GENeSYS_MOD.data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81D135AD-9A63-467D-BAB5-DA91BB083ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06E4F92-9222-4EB9-8BED-E37A287C0B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="38616" windowHeight="21096" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Storage_selection!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$154</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$156</definedName>
     <definedName name="Fuels">#REF!</definedName>
     <definedName name="Technologies">#REF!:B</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="295">
   <si>
     <t>DE</t>
   </si>
@@ -926,6 +926,15 @@
   </si>
   <si>
     <t>Heat_MediumHigh_Industrial</t>
+  </si>
+  <si>
+    <t>CHP_WasteToEnergy</t>
+  </si>
+  <si>
+    <t>R_Waste</t>
+  </si>
+  <si>
+    <t>Waste</t>
   </si>
 </sst>
 </file>
@@ -1291,16 +1300,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A667788-FC3C-4C43-9E46-ED47A2AEE749}">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>205</v>
       </c>
@@ -1309,7 +1318,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>209</v>
       </c>
@@ -1318,7 +1327,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1326,7 +1335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1334,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1342,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1350,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1358,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1366,7 +1375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1374,7 +1383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1382,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1390,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1398,7 +1407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1406,7 +1415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1414,7 +1423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1422,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1430,7 +1439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1438,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1446,7 +1455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1454,7 +1463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1462,7 +1471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1470,7 +1479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1478,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1486,7 +1495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1494,7 +1503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1502,7 +1511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1510,7 +1519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1518,7 +1527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1534,7 +1543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1542,7 +1551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1550,7 +1559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1558,7 +1567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1566,7 +1575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1574,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1590,7 +1599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1598,7 +1607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>210</v>
       </c>
@@ -1606,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -1614,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>212</v>
       </c>
@@ -1622,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>213</v>
       </c>
@@ -1630,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>214</v>
       </c>
@@ -1638,7 +1647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>215</v>
       </c>
@@ -1646,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>216</v>
       </c>
@@ -1654,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>217</v>
       </c>
@@ -1662,7 +1671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>218</v>
       </c>
@@ -1670,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>219</v>
       </c>
@@ -1678,7 +1687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>220</v>
       </c>
@@ -1686,7 +1695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>221</v>
       </c>
@@ -1694,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -1702,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>223</v>
       </c>
@@ -1710,7 +1719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>224</v>
       </c>
@@ -1718,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>225</v>
       </c>
@@ -1726,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>226</v>
       </c>
@@ -1734,7 +1743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>227</v>
       </c>
@@ -1749,18 +1758,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B154"/>
+  <dimension ref="A1:B156"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="F97" sqref="F97"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>135</v>
       </c>
@@ -1768,7 +1777,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1776,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1784,7 +1793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1792,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1800,7 +1809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1808,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1816,7 +1825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1824,7 +1833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1832,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1840,7 +1849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1848,7 +1857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1856,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1864,7 +1873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1880,7 +1889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1888,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1896,1110 +1905,1126 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>292</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>53</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>54</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>55</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>56</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>57</v>
       </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>279</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>280</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>281</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>58</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
         <v>59</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>232</v>
       </c>
-      <c r="B39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>233</v>
       </c>
-      <c r="B40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>234</v>
       </c>
-      <c r="B41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>235</v>
       </c>
-      <c r="B42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>236</v>
       </c>
-      <c r="B43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="B44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>237</v>
       </c>
-      <c r="B44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>238</v>
       </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>239</v>
       </c>
-      <c r="B46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="B47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>240</v>
       </c>
-      <c r="B47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>241</v>
       </c>
-      <c r="B48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>242</v>
       </c>
-      <c r="B49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>243</v>
       </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>285</v>
       </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>286</v>
       </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>287</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>288</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>289</v>
       </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="B56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>72</v>
       </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>73</v>
       </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="B58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>74</v>
       </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="B59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>75</v>
       </c>
-      <c r="B59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>76</v>
       </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="B61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>77</v>
       </c>
-      <c r="B61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>78</v>
       </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="B63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>79</v>
       </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="B64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>80</v>
       </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="B65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>71</v>
       </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="B66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>81</v>
       </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>82</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>83</v>
       </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>84</v>
       </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="B70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>85</v>
       </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="B71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>86</v>
       </c>
-      <c r="B71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="B72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>87</v>
       </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="B73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>88</v>
       </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="B74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>89</v>
       </c>
-      <c r="B74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="B75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>269</v>
       </c>
-      <c r="B75">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="B76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>270</v>
       </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>271</v>
       </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="B78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
         <v>272</v>
       </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>273</v>
       </c>
-      <c r="B79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="B80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
         <v>274</v>
       </c>
-      <c r="B80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>275</v>
       </c>
-      <c r="B81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>276</v>
       </c>
-      <c r="B82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="B83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
         <v>277</v>
       </c>
-      <c r="B83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="B84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>90</v>
       </c>
-      <c r="B84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>91</v>
       </c>
-      <c r="B85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="B86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>92</v>
       </c>
-      <c r="B86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
         <v>93</v>
       </c>
-      <c r="B87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>94</v>
       </c>
-      <c r="B88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="B89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
         <v>95</v>
       </c>
-      <c r="B89">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="B90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
         <v>250</v>
       </c>
-      <c r="B90">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
         <v>96</v>
       </c>
-      <c r="B91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="B92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>99</v>
       </c>
-      <c r="B92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="B93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>97</v>
       </c>
-      <c r="B93">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
         <v>98</v>
       </c>
-      <c r="B94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>251</v>
       </c>
-      <c r="B95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="B96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
         <v>100</v>
       </c>
-      <c r="B96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>266</v>
       </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="B98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>267</v>
       </c>
-      <c r="B98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="B99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
         <v>101</v>
       </c>
-      <c r="B99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>252</v>
       </c>
-      <c r="B100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>102</v>
       </c>
-      <c r="B101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
         <v>253</v>
       </c>
-      <c r="B102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="B103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
         <v>254</v>
       </c>
-      <c r="B103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="B104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>255</v>
       </c>
-      <c r="B104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>256</v>
       </c>
-      <c r="B105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
         <v>257</v>
       </c>
-      <c r="B106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
         <v>258</v>
       </c>
-      <c r="B107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="B108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
         <v>259</v>
       </c>
-      <c r="B108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="B109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
         <v>260</v>
       </c>
-      <c r="B109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="B110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
         <v>261</v>
       </c>
-      <c r="B110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
         <v>262</v>
       </c>
-      <c r="B111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="B112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>263</v>
       </c>
-      <c r="B112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
         <v>264</v>
       </c>
-      <c r="B113">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+      <c r="B114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
+      <c r="B115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
+      <c r="B122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B122">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
+      <c r="B123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="B124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
         <v>244</v>
       </c>
-      <c r="B124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="B125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
         <v>113</v>
       </c>
-      <c r="B125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="B126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
         <v>114</v>
       </c>
-      <c r="B126">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="B127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
         <v>115</v>
       </c>
-      <c r="B127">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="B128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
         <v>245</v>
       </c>
-      <c r="B128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="B129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
         <v>116</v>
       </c>
-      <c r="B129">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="B130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
         <v>117</v>
       </c>
-      <c r="B130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="B131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
         <v>246</v>
       </c>
-      <c r="B131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="B132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
         <v>247</v>
       </c>
-      <c r="B132">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="B133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
         <v>248</v>
       </c>
-      <c r="B133">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>293</v>
+      </c>
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
         <v>249</v>
       </c>
-      <c r="B134">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
         <v>228</v>
       </c>
-      <c r="B135">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
         <v>231</v>
       </c>
-      <c r="B136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="B138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>118</v>
       </c>
-      <c r="B137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
+      <c r="B139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A140" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" t="s">
         <v>278</v>
       </c>
-      <c r="B140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="2" t="s">
+      <c r="B142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A143" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+      <c r="B143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A144" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="B144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A145" t="s">
         <v>123</v>
       </c>
-      <c r="B143">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+      <c r="B145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A146" t="s">
         <v>229</v>
       </c>
-      <c r="B144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="B146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A147" t="s">
         <v>124</v>
       </c>
-      <c r="B145">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="B147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A148" t="s">
         <v>125</v>
       </c>
-      <c r="B146">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="B148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A149" t="s">
         <v>230</v>
       </c>
-      <c r="B147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="B149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A150" t="s">
         <v>126</v>
       </c>
-      <c r="B148">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="B150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A151" t="s">
         <v>127</v>
       </c>
-      <c r="B149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="B151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A152" t="s">
         <v>128</v>
       </c>
-      <c r="B150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="2" t="s">
+      <c r="B152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A153" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="B153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A154" t="s">
         <v>130</v>
       </c>
-      <c r="B152">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="B154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A155" t="s">
         <v>131</v>
       </c>
-      <c r="B153">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="B155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A156" t="s">
         <v>132</v>
       </c>
-      <c r="B154">
+      <c r="B156">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B154" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B154">
-      <sortCondition ref="A1:A154"/>
+  <autoFilter ref="A1:B156" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B156">
+      <sortCondition ref="A1:A156"/>
     </sortState>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A68 A31:A34 A144 A16:A17" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A69 A32:A35 A146 A16:A18" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -3015,12 +3040,12 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>170</v>
       </c>
@@ -3028,7 +3053,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>173</v>
       </c>
@@ -3036,7 +3061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -3044,7 +3069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>175</v>
       </c>
@@ -3052,7 +3077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>172</v>
       </c>
@@ -3060,7 +3085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -3068,7 +3093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>282</v>
       </c>
@@ -3076,7 +3101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>284</v>
       </c>
@@ -3084,7 +3109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>283</v>
       </c>
@@ -3092,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>171</v>
       </c>
@@ -3112,18 +3137,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>138</v>
       </c>
@@ -3131,7 +3156,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -3139,7 +3164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>139</v>
       </c>
@@ -3147,7 +3172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>140</v>
       </c>
@@ -3155,7 +3180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>156</v>
       </c>
@@ -3163,7 +3188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -3171,7 +3196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>163</v>
       </c>
@@ -3179,7 +3204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -3187,7 +3212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -3195,7 +3220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>151</v>
       </c>
@@ -3203,7 +3228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -3211,7 +3236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>152</v>
       </c>
@@ -3219,7 +3244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>143</v>
       </c>
@@ -3227,7 +3252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>268</v>
       </c>
@@ -3235,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -3243,7 +3268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>265</v>
       </c>
@@ -3251,7 +3276,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>166</v>
       </c>
@@ -3259,7 +3284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -3267,7 +3292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>153</v>
       </c>
@@ -3275,7 +3300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>154</v>
       </c>
@@ -3283,7 +3308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>290</v>
       </c>
@@ -3291,7 +3316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>291</v>
       </c>
@@ -3299,7 +3324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>159</v>
       </c>
@@ -3307,7 +3332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>161</v>
       </c>
@@ -3315,7 +3340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>150</v>
       </c>
@@ -3323,7 +3348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>158</v>
       </c>
@@ -3331,7 +3356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>160</v>
       </c>
@@ -3339,7 +3364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>148</v>
       </c>
@@ -3347,7 +3372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -3355,7 +3380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>145</v>
       </c>
@@ -3363,7 +3388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>146</v>
       </c>
@@ -3371,7 +3396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>147</v>
       </c>
@@ -3379,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>157</v>
       </c>
@@ -3387,11 +3412,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>157</v>
       </c>
       <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>294</v>
+      </c>
+      <c r="B35">
         <v>1</v>
       </c>
     </row>
@@ -3419,9 +3452,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>168</v>
       </c>
@@ -3429,7 +3462,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3437,7 +3470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3445,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3453,7 +3486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3461,7 +3494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3469,7 +3502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3490,9 +3523,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
@@ -3500,7 +3533,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>134</v>
       </c>
@@ -3521,9 +3554,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>208</v>
       </c>
@@ -3531,7 +3564,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>178</v>
       </c>
@@ -3539,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -3547,7 +3580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -3555,7 +3588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -3563,7 +3596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -3571,7 +3604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>183</v>
       </c>
@@ -3579,7 +3612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -3587,7 +3620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -3595,7 +3628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>186</v>
       </c>
@@ -3603,7 +3636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>187</v>
       </c>
@@ -3611,7 +3644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>188</v>
       </c>
@@ -3619,7 +3652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>189</v>
       </c>
@@ -3627,7 +3660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>190</v>
       </c>
@@ -3635,7 +3668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>191</v>
       </c>
@@ -3643,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>192</v>
       </c>
@@ -3651,7 +3684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>193</v>
       </c>
@@ -3659,7 +3692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>194</v>
       </c>
@@ -3667,7 +3700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>195</v>
       </c>
@@ -3688,9 +3721,9 @@
       <selection activeCell="Q37" sqref="Q37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>207</v>
       </c>
@@ -3698,7 +3731,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>147</v>
       </c>
@@ -3706,7 +3739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>197</v>
       </c>
@@ -3714,7 +3747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>198</v>
       </c>
@@ -3722,7 +3755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>199</v>
       </c>
@@ -3730,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>200</v>
       </c>
@@ -3738,7 +3771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>201</v>
       </c>
@@ -3746,7 +3779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>202</v>
       </c>
@@ -3754,7 +3787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>203</v>
       </c>
@@ -3775,9 +3808,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>206</v>
       </c>
@@ -3786,7 +3819,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -3794,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -3802,7 +3835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -3810,7 +3843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -3818,7 +3851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -3826,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -3834,7 +3867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -3842,7 +3875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2035</v>
       </c>
@@ -3850,7 +3883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2040</v>
       </c>
@@ -3858,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2045</v>
       </c>
@@ -3866,7 +3899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2050</v>
       </c>
@@ -3874,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2055</v>
       </c>
@@ -3882,7 +3915,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2060</v>
       </c>

</xml_diff>

<commit_message>
Improved district heat formulation: Added new parameters: DistrictHeatDemand; DistrictHeatSplit (to distinguish between buildings and industry consumption) Combined Convert_DH technologies to one technology "X_Convert_HD" with two modes of operation
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06E4F92-9222-4EB9-8BED-E37A287C0B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D06339-77B9-4D6F-9A16-7AB751A3171E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="38616" windowHeight="21096" activeTab="3" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="38292" yWindow="-108" windowWidth="29016" windowHeight="15696" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Storage_selection!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$156</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$155</definedName>
     <definedName name="Fuels">#REF!</definedName>
     <definedName name="Technologies">#REF!:B</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="294">
   <si>
     <t>DE</t>
   </si>
@@ -265,9 +265,6 @@
     <t>FRT_Ship_LNG</t>
   </si>
   <si>
-    <t>HLI_Convert_DH</t>
-  </si>
-  <si>
     <t>HHI_BF_BOF</t>
   </si>
   <si>
@@ -751,9 +748,6 @@
     <t>HB_Biomass</t>
   </si>
   <si>
-    <t>HB_Convert_DH</t>
-  </si>
-  <si>
     <t>HB_Direct_Electric</t>
   </si>
   <si>
@@ -935,6 +929,9 @@
   </si>
   <si>
     <t>Waste</t>
+  </si>
+  <si>
+    <t>X_Convert_HD</t>
   </si>
 </sst>
 </file>
@@ -1311,7 +1308,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1320,7 +1317,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1609,7 +1606,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1617,7 +1614,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1625,7 +1622,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1633,7 +1630,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1641,7 +1638,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1649,7 +1646,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1657,7 +1654,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1665,7 +1662,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1673,7 +1670,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1681,7 +1678,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1689,7 +1686,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1697,7 +1694,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1705,7 +1702,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1713,7 +1710,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1721,7 +1718,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1729,7 +1726,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1737,7 +1734,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1745,7 +1742,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1758,10 +1755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B156"/>
+  <dimension ref="A1:B155"/>
   <sheetViews>
-    <sheetView topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1771,10 +1768,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1907,7 +1904,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1955,7 +1952,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1963,7 +1960,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1971,7 +1968,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2083,7 +2080,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2091,7 +2088,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2099,7 +2096,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2107,7 +2104,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2115,7 +2112,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2123,7 +2120,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2131,7 +2128,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2139,7 +2136,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2147,7 +2144,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2155,7 +2152,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2163,7 +2160,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2171,7 +2168,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2179,7 +2176,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2187,7 +2184,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2195,7 +2192,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2203,7 +2200,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -2211,7 +2208,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>289</v>
+        <v>71</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -2291,7 +2288,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2299,7 +2296,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -2307,7 +2304,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -2315,7 +2312,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -2323,7 +2320,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2331,7 +2328,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2339,7 +2336,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2347,7 +2344,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2355,7 +2352,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>88</v>
+        <v>267</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2363,7 +2360,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>89</v>
+        <v>268</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2427,7 +2424,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>276</v>
+        <v>89</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2435,7 +2432,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>277</v>
+        <v>90</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2443,7 +2440,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -2451,7 +2448,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2459,7 +2456,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B87">
         <v>1</v>
@@ -2467,7 +2464,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2475,7 +2472,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>94</v>
+        <v>248</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2491,7 +2488,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>250</v>
+        <v>98</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2507,7 +2504,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2515,7 +2512,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>249</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2523,7 +2520,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2531,7 +2528,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2539,7 +2536,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>100</v>
+        <v>265</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2547,7 +2544,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>266</v>
+        <v>100</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2555,7 +2552,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2571,7 +2568,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -2579,7 +2576,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>252</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -2666,16 +2663,16 @@
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>263</v>
+      <c r="A113" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B113">
         <v>1</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>264</v>
+      <c r="A114" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -2683,7 +2680,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -2691,7 +2688,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -2699,7 +2696,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B117">
         <v>1</v>
@@ -2707,7 +2704,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B118">
         <v>1</v>
@@ -2715,7 +2712,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -2723,7 +2720,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B120">
         <v>1</v>
@@ -2731,7 +2728,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -2739,22 +2736,22 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B122">
         <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
-        <v>111</v>
+      <c r="A123" t="s">
+        <v>242</v>
       </c>
       <c r="B123">
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
+      <c r="A124" t="s">
         <v>112</v>
       </c>
       <c r="B124">
@@ -2763,7 +2760,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>244</v>
+        <v>113</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2771,7 +2768,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2779,7 +2776,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>114</v>
+        <v>243</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2795,7 +2792,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>245</v>
+        <v>116</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2803,7 +2800,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>116</v>
+        <v>244</v>
       </c>
       <c r="B130">
         <v>1</v>
@@ -2811,7 +2808,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>117</v>
+        <v>245</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -2827,7 +2824,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>247</v>
+        <v>291</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2835,7 +2832,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -2843,7 +2840,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>293</v>
+        <v>227</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2851,7 +2848,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2859,7 +2856,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>228</v>
+        <v>117</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -2867,14 +2864,14 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>231</v>
+        <v>293</v>
       </c>
       <c r="B138">
         <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
+      <c r="A139" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B139">
@@ -2890,16 +2887,16 @@
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="2" t="s">
+      <c r="A141" t="s">
+        <v>276</v>
+      </c>
+      <c r="B141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A142" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B141">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" t="s">
-        <v>278</v>
       </c>
       <c r="B142">
         <v>1</v>
@@ -2914,7 +2911,7 @@
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="2" t="s">
+      <c r="A144" t="s">
         <v>122</v>
       </c>
       <c r="B144">
@@ -2923,7 +2920,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>123</v>
+        <v>228</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2931,7 +2928,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>229</v>
+        <v>123</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -2947,7 +2944,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>125</v>
+        <v>229</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2955,7 +2952,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>230</v>
+        <v>125</v>
       </c>
       <c r="B149">
         <v>1</v>
@@ -2978,7 +2975,7 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" t="s">
+      <c r="A152" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B152">
@@ -2986,7 +2983,7 @@
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="2" t="s">
+      <c r="A153" t="s">
         <v>129</v>
       </c>
       <c r="B153">
@@ -3009,22 +3006,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" t="s">
-        <v>132</v>
-      </c>
-      <c r="B156">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B156" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B156">
-      <sortCondition ref="A1:A156"/>
+  <autoFilter ref="A1:B155" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B155">
+      <sortCondition ref="A1:A155"/>
     </sortState>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A69 A32:A35 A146 A16:A18" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A67 A32:A35 A145 A16:A18" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -3047,15 +3036,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3063,7 +3052,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3071,7 +3060,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3079,7 +3068,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3087,7 +3076,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3095,7 +3084,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3103,7 +3092,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3111,7 +3100,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3119,7 +3108,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3139,7 +3128,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7942D6-5BBA-4326-BEB2-07D45E712A14}">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -3150,15 +3139,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3166,7 +3155,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3174,7 +3163,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3182,7 +3171,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3190,7 +3179,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3198,7 +3187,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3206,7 +3195,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3214,7 +3203,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3222,7 +3211,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3230,7 +3219,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3238,7 +3227,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3246,7 +3235,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3254,7 +3243,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3262,7 +3251,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3270,7 +3259,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3278,7 +3267,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3286,7 +3275,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3294,7 +3283,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3302,7 +3291,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3310,7 +3299,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3318,7 +3307,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3326,7 +3315,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3334,7 +3323,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3342,7 +3331,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3350,7 +3339,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3358,7 +3347,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3366,7 +3355,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3374,7 +3363,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3382,7 +3371,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3390,7 +3379,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3398,7 +3387,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3406,7 +3395,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3414,7 +3403,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3422,7 +3411,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -3456,10 +3445,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3527,15 +3516,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3558,15 +3547,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3574,7 +3563,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3582,7 +3571,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3590,7 +3579,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3598,7 +3587,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3606,7 +3595,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3614,7 +3603,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3622,7 +3611,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3630,7 +3619,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3638,7 +3627,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3646,7 +3635,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3654,7 +3643,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3662,7 +3651,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3670,7 +3659,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3678,7 +3667,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3686,7 +3675,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3694,7 +3683,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3702,7 +3691,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3725,15 +3714,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3741,7 +3730,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3749,7 +3738,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3757,7 +3746,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3765,7 +3754,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3773,7 +3762,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3781,7 +3770,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3789,7 +3778,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3812,7 +3801,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
fixed some mistakes in removal of a technology
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D06339-77B9-4D6F-9A16-7AB751A3171E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CED16B-5924-4F60-BC18-89A97EF5C97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38292" yWindow="-108" windowWidth="29016" windowHeight="15696" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="38292" yWindow="-108" windowWidth="38616" windowHeight="21096" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Storage_selection!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$155</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Technology_selection!$A$1:$B$154</definedName>
     <definedName name="Fuels">#REF!</definedName>
     <definedName name="Technologies">#REF!:B</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="293">
   <si>
     <t>DE</t>
   </si>
@@ -293,9 +293,6 @@
   </si>
   <si>
     <t>HLI_Direct_Electric</t>
-  </si>
-  <si>
-    <t>HLI_Fuelcell</t>
   </si>
   <si>
     <t>HLI_Gas_Boiler</t>
@@ -1308,7 +1305,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>7</v>
@@ -1317,7 +1314,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1606,7 +1603,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -1614,7 +1611,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -1622,7 +1619,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -1630,7 +1627,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1638,7 +1635,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -1646,7 +1643,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1654,7 +1651,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1662,7 +1659,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1670,7 +1667,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1678,7 +1675,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1686,7 +1683,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -1694,7 +1691,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1702,7 +1699,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1710,7 +1707,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1718,7 +1715,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1726,7 +1723,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1734,7 +1731,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1742,7 +1739,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -1755,10 +1752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
-  <dimension ref="A1:B155"/>
+  <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1768,10 +1765,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1904,7 +1901,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -1952,7 +1949,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1960,7 +1957,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1968,7 +1965,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -2080,7 +2077,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -2088,7 +2085,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -2096,7 +2093,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -2104,7 +2101,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2112,7 +2109,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -2120,7 +2117,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B45">
         <v>1</v>
@@ -2128,7 +2125,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2136,7 +2133,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -2144,7 +2141,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -2152,7 +2149,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -2160,7 +2157,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -2168,7 +2165,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -2176,7 +2173,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -2184,7 +2181,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -2192,7 +2189,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B54">
         <v>1</v>
@@ -2200,7 +2197,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B55">
         <v>1</v>
@@ -2344,7 +2341,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>266</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2416,7 +2413,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>275</v>
+        <v>88</v>
       </c>
       <c r="B82">
         <v>1</v>
@@ -2464,7 +2461,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>247</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -2472,7 +2469,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>248</v>
+        <v>94</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -2480,7 +2477,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -2488,7 +2485,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B91">
         <v>1</v>
@@ -2504,7 +2501,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>97</v>
+        <v>248</v>
       </c>
       <c r="B93">
         <v>1</v>
@@ -2512,7 +2509,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>249</v>
+        <v>98</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -2520,7 +2517,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>99</v>
+        <v>263</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -2536,7 +2533,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>265</v>
+        <v>99</v>
       </c>
       <c r="B97">
         <v>1</v>
@@ -2544,7 +2541,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>100</v>
+        <v>249</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2552,7 +2549,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2560,7 +2557,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>250</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -2655,8 +2652,8 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>262</v>
+      <c r="A112" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2735,8 +2732,8 @@
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
-        <v>111</v>
+      <c r="A122" t="s">
+        <v>241</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2744,7 +2741,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>242</v>
+        <v>111</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2768,7 +2765,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>114</v>
+        <v>242</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -2776,7 +2773,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>243</v>
+        <v>114</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2792,7 +2789,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>116</v>
+        <v>243</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2816,7 +2813,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>246</v>
+        <v>290</v>
       </c>
       <c r="B132">
         <v>1</v>
@@ -2824,7 +2821,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>291</v>
+        <v>246</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2832,7 +2829,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="B134">
         <v>1</v>
@@ -2840,7 +2837,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2848,7 +2845,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>230</v>
+        <v>116</v>
       </c>
       <c r="B136">
         <v>1</v>
@@ -2856,15 +2853,15 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
+        <v>292</v>
+      </c>
+      <c r="B137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" s="2" t="s">
         <v>117</v>
-      </c>
-      <c r="B137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" t="s">
-        <v>293</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2879,16 +2876,16 @@
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="2" t="s">
+      <c r="A140" t="s">
+        <v>275</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A141" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" t="s">
-        <v>276</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2903,7 +2900,7 @@
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="2" t="s">
+      <c r="A143" t="s">
         <v>121</v>
       </c>
       <c r="B143">
@@ -2912,7 +2909,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>122</v>
+        <v>227</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -2920,7 +2917,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>228</v>
+        <v>122</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2936,7 +2933,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>124</v>
+        <v>228</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2944,7 +2941,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>229</v>
+        <v>124</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2967,7 +2964,7 @@
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
+      <c r="A151" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B151">
@@ -2975,7 +2972,7 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="2" t="s">
+      <c r="A152" t="s">
         <v>128</v>
       </c>
       <c r="B152">
@@ -2995,14 +2992,6 @@
         <v>130</v>
       </c>
       <c r="B154">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" t="s">
-        <v>131</v>
-      </c>
-      <c r="B155">
         <v>1</v>
       </c>
     </row>
@@ -3013,7 +3002,7 @@
     </sortState>
   </autoFilter>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A67 A32:A35 A145 A16:A18" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A66 A32:A35 A144 A16:A18" xr:uid="{F3A41512-0F1A-4AAA-A425-8857F9308381}">
       <formula1>Technologies</formula1>
     </dataValidation>
   </dataValidations>
@@ -3036,15 +3025,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3052,7 +3041,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3060,7 +3049,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3068,7 +3057,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3076,7 +3065,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3084,7 +3073,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3092,7 +3081,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3100,7 +3089,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3108,7 +3097,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3139,15 +3128,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3155,7 +3144,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3163,7 +3152,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3171,7 +3160,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3179,7 +3168,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3187,7 +3176,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3195,7 +3184,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3203,7 +3192,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3211,7 +3200,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3219,7 +3208,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3227,7 +3216,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3235,7 +3224,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3243,7 +3232,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3251,7 +3240,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3259,7 +3248,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3267,7 +3256,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3275,7 +3264,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3283,7 +3272,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3291,7 +3280,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3299,7 +3288,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3307,7 +3296,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -3315,7 +3304,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3323,7 +3312,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -3331,7 +3320,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -3339,7 +3328,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3347,7 +3336,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3355,7 +3344,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3363,7 +3352,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3371,7 +3360,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3379,7 +3368,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3387,7 +3376,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3395,7 +3384,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3403,7 +3392,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3411,7 +3400,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -3445,10 +3434,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -3516,15 +3505,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3547,15 +3536,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3563,7 +3552,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3571,7 +3560,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3579,7 +3568,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3587,7 +3576,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3595,7 +3584,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3603,7 +3592,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3611,7 +3600,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3619,7 +3608,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -3627,7 +3616,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -3635,7 +3624,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -3643,7 +3632,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -3651,7 +3640,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -3659,7 +3648,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -3667,7 +3656,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -3675,7 +3664,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -3683,7 +3672,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -3691,7 +3680,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3714,15 +3703,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3730,7 +3719,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3738,7 +3727,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3746,7 +3735,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -3754,7 +3743,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -3762,7 +3751,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3770,7 +3759,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -3778,7 +3767,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -3801,7 +3790,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
added new sector "DistrictHeating" and updated relevant entries
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CED16B-5924-4F60-BC18-89A97EF5C97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD01708A-CAF4-4675-872B-CF0886210EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38292" yWindow="-108" windowWidth="38616" windowHeight="21096" activeTab="1" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="294">
   <si>
     <t>DE</t>
   </si>
@@ -929,6 +929,9 @@
   </si>
   <si>
     <t>X_Convert_HD</t>
+  </si>
+  <si>
+    <t>DistrictHeating</t>
   </si>
 </sst>
 </file>
@@ -1298,12 +1301,12 @@
       <selection activeCell="B2" sqref="B2:B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>203</v>
       </c>
@@ -1312,7 +1315,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>207</v>
       </c>
@@ -1321,7 +1324,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1329,7 +1332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1337,7 +1340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1345,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1353,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1361,7 +1364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1377,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1385,7 +1388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1401,7 +1404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1409,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1433,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1457,7 +1460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1465,7 +1468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1473,7 +1476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1489,7 +1492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1505,7 +1508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1513,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1521,7 +1524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1529,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1545,7 +1548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1553,7 +1556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1569,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1577,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1593,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>208</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>209</v>
       </c>
@@ -1617,7 +1620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>210</v>
       </c>
@@ -1625,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>211</v>
       </c>
@@ -1633,7 +1636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>212</v>
       </c>
@@ -1641,7 +1644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>213</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>214</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>215</v>
       </c>
@@ -1665,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>216</v>
       </c>
@@ -1673,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>217</v>
       </c>
@@ -1681,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>218</v>
       </c>
@@ -1689,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -1697,7 +1700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>220</v>
       </c>
@@ -1705,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -1713,7 +1716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>222</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -1737,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -1754,16 +1757,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5D2E10-6D88-4A1E-9C1A-BD9E15FD6A9D}">
   <dimension ref="A1:B154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A36" workbookViewId="0">
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
@@ -1771,7 +1774,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1779,7 +1782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1795,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1819,7 +1822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1827,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1835,7 +1838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1843,7 +1846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1851,7 +1854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1867,7 +1870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1875,7 +1878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1883,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1891,7 +1894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1899,7 +1902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>289</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1915,7 +1918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1923,7 +1926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1931,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -1939,7 +1942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1947,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>276</v>
       </c>
@@ -1955,7 +1958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>277</v>
       </c>
@@ -1963,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>278</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1979,7 +1982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>60</v>
       </c>
@@ -1995,7 +1998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
@@ -2003,7 +2006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
@@ -2011,7 +2014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -2019,7 +2022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
@@ -2035,7 +2038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -2043,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -2051,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
@@ -2059,7 +2062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>69</v>
       </c>
@@ -2067,7 +2070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>70</v>
       </c>
@@ -2075,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>230</v>
       </c>
@@ -2083,7 +2086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>231</v>
       </c>
@@ -2091,7 +2094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>232</v>
       </c>
@@ -2099,7 +2102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>233</v>
       </c>
@@ -2107,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>234</v>
       </c>
@@ -2115,7 +2118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -2123,7 +2126,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>236</v>
       </c>
@@ -2131,7 +2134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>237</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>238</v>
       </c>
@@ -2147,7 +2150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>239</v>
       </c>
@@ -2155,7 +2158,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>240</v>
       </c>
@@ -2163,7 +2166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>282</v>
       </c>
@@ -2171,7 +2174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>283</v>
       </c>
@@ -2179,7 +2182,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>284</v>
       </c>
@@ -2187,7 +2190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>285</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>286</v>
       </c>
@@ -2203,7 +2206,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -2211,7 +2214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -2219,7 +2222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -2227,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -2235,7 +2238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -2243,7 +2246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -2251,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -2259,7 +2262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -2267,7 +2270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -2275,7 +2278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -2283,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -2291,7 +2294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -2299,7 +2302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -2307,7 +2310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -2315,7 +2318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -2331,7 +2334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -2339,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>266</v>
       </c>
@@ -2347,7 +2350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>267</v>
       </c>
@@ -2355,7 +2358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>268</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>269</v>
       </c>
@@ -2371,7 +2374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>270</v>
       </c>
@@ -2379,7 +2382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>271</v>
       </c>
@@ -2387,7 +2390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>272</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>273</v>
       </c>
@@ -2403,7 +2406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>274</v>
       </c>
@@ -2411,7 +2414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -2419,7 +2422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -2427,7 +2430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -2435,7 +2438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -2443,7 +2446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -2451,7 +2454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -2459,7 +2462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>247</v>
       </c>
@@ -2467,7 +2470,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -2475,7 +2478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -2483,7 +2486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -2491,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -2499,7 +2502,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>248</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>98</v>
       </c>
@@ -2515,7 +2518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>263</v>
       </c>
@@ -2523,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>264</v>
       </c>
@@ -2531,7 +2534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -2539,7 +2542,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>249</v>
       </c>
@@ -2547,7 +2550,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -2555,7 +2558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>250</v>
       </c>
@@ -2563,7 +2566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>251</v>
       </c>
@@ -2571,7 +2574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>252</v>
       </c>
@@ -2579,7 +2582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>253</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>254</v>
       </c>
@@ -2595,7 +2598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>255</v>
       </c>
@@ -2603,7 +2606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>256</v>
       </c>
@@ -2611,7 +2614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>257</v>
       </c>
@@ -2619,7 +2622,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>258</v>
       </c>
@@ -2627,7 +2630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>259</v>
       </c>
@@ -2635,7 +2638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>260</v>
       </c>
@@ -2643,7 +2646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>261</v>
       </c>
@@ -2651,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>101</v>
       </c>
@@ -2659,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>102</v>
       </c>
@@ -2667,7 +2670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>103</v>
       </c>
@@ -2675,7 +2678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>104</v>
       </c>
@@ -2683,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>105</v>
       </c>
@@ -2691,7 +2694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>106</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>107</v>
       </c>
@@ -2707,7 +2710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>108</v>
       </c>
@@ -2715,7 +2718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>109</v>
       </c>
@@ -2723,7 +2726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>110</v>
       </c>
@@ -2731,7 +2734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>241</v>
       </c>
@@ -2739,7 +2742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>111</v>
       </c>
@@ -2747,7 +2750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>112</v>
       </c>
@@ -2755,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>113</v>
       </c>
@@ -2763,7 +2766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>242</v>
       </c>
@@ -2771,7 +2774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>114</v>
       </c>
@@ -2779,7 +2782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>115</v>
       </c>
@@ -2787,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>243</v>
       </c>
@@ -2795,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>244</v>
       </c>
@@ -2803,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>245</v>
       </c>
@@ -2811,7 +2814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>290</v>
       </c>
@@ -2819,7 +2822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>246</v>
       </c>
@@ -2827,7 +2830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>226</v>
       </c>
@@ -2835,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>229</v>
       </c>
@@ -2843,7 +2846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>116</v>
       </c>
@@ -2851,7 +2854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>292</v>
       </c>
@@ -2859,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>117</v>
       </c>
@@ -2867,7 +2870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>118</v>
       </c>
@@ -2875,7 +2878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>275</v>
       </c>
@@ -2883,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>119</v>
       </c>
@@ -2891,7 +2894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>120</v>
       </c>
@@ -2899,7 +2902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>121</v>
       </c>
@@ -2907,7 +2910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>227</v>
       </c>
@@ -2915,7 +2918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>122</v>
       </c>
@@ -2923,7 +2926,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>123</v>
       </c>
@@ -2931,7 +2934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>228</v>
       </c>
@@ -2939,7 +2942,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>124</v>
       </c>
@@ -2947,7 +2950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>125</v>
       </c>
@@ -2955,7 +2958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>126</v>
       </c>
@@ -2963,7 +2966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>127</v>
       </c>
@@ -2971,7 +2974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>128</v>
       </c>
@@ -2979,7 +2982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>129</v>
       </c>
@@ -2987,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>130</v>
       </c>
@@ -3018,12 +3021,12 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>168</v>
       </c>
@@ -3031,7 +3034,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -3039,7 +3042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -3047,7 +3050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -3055,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>170</v>
       </c>
@@ -3063,7 +3066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -3071,7 +3074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>279</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>281</v>
       </c>
@@ -3087,7 +3090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -3095,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>169</v>
       </c>
@@ -3121,12 +3124,12 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>136</v>
       </c>
@@ -3134,7 +3137,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>160</v>
       </c>
@@ -3142,7 +3145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -3150,7 +3153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -3158,7 +3161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -3166,7 +3169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -3174,7 +3177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -3190,7 +3193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -3198,7 +3201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -3206,7 +3209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -3214,7 +3217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -3222,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3230,7 +3233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>265</v>
       </c>
@@ -3238,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -3246,7 +3249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>262</v>
       </c>
@@ -3254,7 +3257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>164</v>
       </c>
@@ -3262,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>153</v>
       </c>
@@ -3270,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -3278,7 +3281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -3286,7 +3289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>287</v>
       </c>
@@ -3294,7 +3297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>288</v>
       </c>
@@ -3302,7 +3305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>157</v>
       </c>
@@ -3310,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>159</v>
       </c>
@@ -3318,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -3334,7 +3337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>158</v>
       </c>
@@ -3342,7 +3345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -3350,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>147</v>
       </c>
@@ -3358,7 +3361,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -3374,7 +3377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -3382,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>155</v>
       </c>
@@ -3390,7 +3393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -3398,7 +3401,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>291</v>
       </c>
@@ -3430,9 +3433,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>166</v>
       </c>
@@ -3440,7 +3443,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3448,7 +3451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3456,7 +3459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3464,7 +3467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3472,7 +3475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3480,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3501,9 +3504,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -3511,7 +3514,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -3532,9 +3535,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>206</v>
       </c>
@@ -3542,7 +3545,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -3550,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -3558,7 +3561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -3566,7 +3569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>179</v>
       </c>
@@ -3574,7 +3577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>180</v>
       </c>
@@ -3582,7 +3585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -3590,7 +3593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>182</v>
       </c>
@@ -3598,7 +3601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>183</v>
       </c>
@@ -3606,7 +3609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>184</v>
       </c>
@@ -3614,7 +3617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -3622,7 +3625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>186</v>
       </c>
@@ -3630,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>187</v>
       </c>
@@ -3638,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>188</v>
       </c>
@@ -3646,7 +3649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>189</v>
       </c>
@@ -3654,7 +3657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>190</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>191</v>
       </c>
@@ -3670,7 +3673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>192</v>
       </c>
@@ -3678,7 +3681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>193</v>
       </c>
@@ -3693,15 +3696,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D5B3E0-498C-4AB7-BB30-7BCE295E19AC}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q37" sqref="Q37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>205</v>
       </c>
@@ -3709,7 +3712,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>145</v>
       </c>
@@ -3717,7 +3720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>195</v>
       </c>
@@ -3725,7 +3728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>196</v>
       </c>
@@ -3733,7 +3736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>197</v>
       </c>
@@ -3741,7 +3744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>199</v>
       </c>
@@ -3757,7 +3760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>200</v>
       </c>
@@ -3765,11 +3768,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>201</v>
       </c>
       <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>293</v>
+      </c>
+      <c r="B10">
         <v>1</v>
       </c>
     </row>
@@ -3786,9 +3797,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>204</v>
       </c>
@@ -3797,7 +3808,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -3805,7 +3816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -3813,7 +3824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -3821,7 +3832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -3829,7 +3840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -3837,7 +3848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -3845,7 +3856,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -3853,7 +3864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2035</v>
       </c>
@@ -3861,7 +3872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2040</v>
       </c>
@@ -3869,7 +3880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2045</v>
       </c>
@@ -3877,7 +3888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2050</v>
       </c>
@@ -3885,7 +3896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2055</v>
       </c>
@@ -3893,7 +3904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2060</v>
       </c>

</xml_diff>

<commit_message>
Add functionality to handle small numeric values using configurable thresholds. Thresholds and replacement values can now be set individually per parameter via the set filter file.
</commit_message>
<xml_diff>
--- a/Conversion Script/Set_filter_file.xlsx
+++ b/Conversion Script/Set_filter_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nim\Documents\GENeSYS_MOD.data\Conversion Script\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jb\GENeSYS_MOD.data\Conversion Script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD01708A-CAF4-4675-872B-CF0886210EA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805B50C3-8859-4C20-88E2-044E3AFC19E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="6" activeTab="9" xr2:uid="{0B764928-35F8-4A30-ADCD-C0369050184D}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_selection" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Modal_type_selection" sheetId="9" r:id="rId7"/>
     <sheet name="Sector_selection" sheetId="10" r:id="rId8"/>
     <sheet name="Year_selection" sheetId="4" r:id="rId9"/>
+    <sheet name="Rounding_thresholds" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Storage_selection!$A$1:$B$1</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="371">
   <si>
     <t>DE</t>
   </si>
@@ -932,6 +933,237 @@
   </si>
   <si>
     <t>DistrictHeating</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Replace with</t>
+  </si>
+  <si>
+    <t>Par_AnnualEmissionLimit</t>
+  </si>
+  <si>
+    <t>Par_AnnualExogenousEmission</t>
+  </si>
+  <si>
+    <t>Par_AnnualMaxNewCapacity</t>
+  </si>
+  <si>
+    <t>Par_AnnualMinNewCapacity</t>
+  </si>
+  <si>
+    <t>Par_AnnualSectoralEmissionLimit</t>
+  </si>
+  <si>
+    <t>Par_AvailabilityFactor</t>
+  </si>
+  <si>
+    <t>Par_BaseYearProduction</t>
+  </si>
+  <si>
+    <t>Par_BaseYearSlack</t>
+  </si>
+  <si>
+    <t>Par_CapacityFactor</t>
+  </si>
+  <si>
+    <t>Par_CapacityToActivityUnit</t>
+  </si>
+  <si>
+    <t>Par_CapitalCost</t>
+  </si>
+  <si>
+    <t>Par_CapitalCostStorage</t>
+  </si>
+  <si>
+    <t>Par_CommissionedTradeCapacity</t>
+  </si>
+  <si>
+    <t>Par_EmissionActivityRatio</t>
+  </si>
+  <si>
+    <t>Par_EmissionContentPerFuel</t>
+  </si>
+  <si>
+    <t>Par_EmissionPenaltyTagTech</t>
+  </si>
+  <si>
+    <t>Par_EmissionsPenalty</t>
+  </si>
+  <si>
+    <t>Par_FixedCost</t>
+  </si>
+  <si>
+    <t>Par_GeneralDiscountRate</t>
+  </si>
+  <si>
+    <t>Par_GrowthRateTradeCapacity</t>
+  </si>
+  <si>
+    <t>Par_InputActivityRatio</t>
+  </si>
+  <si>
+    <t>Par_MinStorageCharge</t>
+  </si>
+  <si>
+    <t>Par_ModalSplitByFuel</t>
+  </si>
+  <si>
+    <t>Par_ModelPeriodActivityMaxLimit</t>
+  </si>
+  <si>
+    <t>Par_ModelPeriodEmissionLimit</t>
+  </si>
+  <si>
+    <t>Par_ModelPeriodExogenousEmission</t>
+  </si>
+  <si>
+    <t>Par_NewCapacityExpansionStop</t>
+  </si>
+  <si>
+    <t>Par_OperationalLife</t>
+  </si>
+  <si>
+    <t>Par_OperationalLifeStorage</t>
+  </si>
+  <si>
+    <t>Par_OutputActivityRatio</t>
+  </si>
+  <si>
+    <t>Par_ProductionChangeCost</t>
+  </si>
+  <si>
+    <t>Par_ProductionGrowthLimit</t>
+  </si>
+  <si>
+    <t>Par_REMinProductionTarget</t>
+  </si>
+  <si>
+    <t>Par_RETagFuel</t>
+  </si>
+  <si>
+    <t>Par_RETagTechnology</t>
+  </si>
+  <si>
+    <t>Par_RampingDownFactor</t>
+  </si>
+  <si>
+    <t>Par_RampingUpFactor</t>
+  </si>
+  <si>
+    <t>Par_RegionalAnnualEmissionLimit</t>
+  </si>
+  <si>
+    <t>Par_RegionalBaseYearProduction</t>
+  </si>
+  <si>
+    <t>Par_RegionalCCSLimit</t>
+  </si>
+  <si>
+    <t>Par_RegionalModelPeriodEmission</t>
+  </si>
+  <si>
+    <t>Par_ReserveMargin</t>
+  </si>
+  <si>
+    <t>Par_ReserveMarginTagFuel</t>
+  </si>
+  <si>
+    <t>Par_ReserveMarginTagTechnology</t>
+  </si>
+  <si>
+    <t>Par_ResidualCapacity</t>
+  </si>
+  <si>
+    <t>Par_ResidualStorageCapacity</t>
+  </si>
+  <si>
+    <t>Par_SelfSufficiency</t>
+  </si>
+  <si>
+    <t>Par_SocialDiscountRate</t>
+  </si>
+  <si>
+    <t>Par_SpecifiedAnnualDemand</t>
+  </si>
+  <si>
+    <t>Par_SpecifiedDemandDevelopment</t>
+  </si>
+  <si>
+    <t>Par_StorageE2PRatio</t>
+  </si>
+  <si>
+    <t>Par_StorageLevelStart</t>
+  </si>
+  <si>
+    <t>Par_TagCanFuelBeTraded</t>
+  </si>
+  <si>
+    <t>Par_TagDemandFuelToSector</t>
+  </si>
+  <si>
+    <t>Par_TagElectricTechnology</t>
+  </si>
+  <si>
+    <t>Par_TagFuelToSubsets</t>
+  </si>
+  <si>
+    <t>Par_TagModalTypeToModalGroups</t>
+  </si>
+  <si>
+    <t>Par_TagTechnologyToModalType</t>
+  </si>
+  <si>
+    <t>Par_TagTechnologyToSector</t>
+  </si>
+  <si>
+    <t>Par_TagTechnologyToSubsets</t>
+  </si>
+  <si>
+    <t>Par_TagTimeIndependentFuel</t>
+  </si>
+  <si>
+    <t>Par_TechnologyDiscountRate</t>
+  </si>
+  <si>
+    <t>Par_TechnologyFromStorage</t>
+  </si>
+  <si>
+    <t>Par_TechnologyToStorage</t>
+  </si>
+  <si>
+    <t>Par_TotalAnnualMaxActivity</t>
+  </si>
+  <si>
+    <t>Par_TotalAnnualMaxCapacity</t>
+  </si>
+  <si>
+    <t>Par_TotalAnnualMinActivity</t>
+  </si>
+  <si>
+    <t>Par_TotalAnnualMinCapacity</t>
+  </si>
+  <si>
+    <t>Par_TradeCapacity</t>
+  </si>
+  <si>
+    <t>Par_TradeCapacityGrowthCosts</t>
+  </si>
+  <si>
+    <t>Par_TradeCostsFactor</t>
+  </si>
+  <si>
+    <t>Par_TradeLossFactor</t>
+  </si>
+  <si>
+    <t>Par_TradeRoute</t>
+  </si>
+  <si>
+    <t>Par_VariableCost</t>
   </si>
 </sst>
 </file>
@@ -975,15 +1207,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -999,9 +1232,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1039,7 +1272,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1145,7 +1378,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1301,12 +1534,12 @@
       <selection activeCell="B2" sqref="B2:B55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>203</v>
       </c>
@@ -1315,7 +1548,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>207</v>
       </c>
@@ -1324,7 +1557,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1332,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1340,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1348,7 +1581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1356,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1364,7 +1597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1372,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1380,7 +1613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1388,7 +1621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1396,7 +1629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1404,7 +1637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1412,7 +1645,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1420,7 +1653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1428,7 +1661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1436,7 +1669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1444,7 +1677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1452,7 +1685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1460,7 +1693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1468,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1476,7 +1709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1484,7 +1717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1492,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1500,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1508,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1516,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1524,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1532,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1540,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1548,7 +1781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1556,7 +1789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1564,7 +1797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1572,7 +1805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1580,7 +1813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1588,7 +1821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1596,7 +1829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1604,7 +1837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>208</v>
       </c>
@@ -1612,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>209</v>
       </c>
@@ -1620,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>210</v>
       </c>
@@ -1628,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>211</v>
       </c>
@@ -1636,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>212</v>
       </c>
@@ -1644,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>213</v>
       </c>
@@ -1652,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>214</v>
       </c>
@@ -1660,7 +1893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>215</v>
       </c>
@@ -1668,7 +1901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>216</v>
       </c>
@@ -1676,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>217</v>
       </c>
@@ -1684,7 +1917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>218</v>
       </c>
@@ -1692,7 +1925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>219</v>
       </c>
@@ -1700,7 +1933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>220</v>
       </c>
@@ -1708,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>221</v>
       </c>
@@ -1716,7 +1949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>222</v>
       </c>
@@ -1724,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>223</v>
       </c>
@@ -1732,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>224</v>
       </c>
@@ -1740,7 +1973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>225</v>
       </c>
@@ -1750,6 +1983,846 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738B5DF0-4614-4AAA-8D30-A109FA3624F2}">
+  <dimension ref="A1:C75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B2" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B4" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>300</v>
+      </c>
+      <c r="B5" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>301</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B7" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>304</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>305</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>306</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>307</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>309</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>311</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>313</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>314</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>315</v>
+      </c>
+      <c r="B20" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>317</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>318</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>319</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>320</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>321</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>322</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>323</v>
+      </c>
+      <c r="B28" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>324</v>
+      </c>
+      <c r="B29" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>325</v>
+      </c>
+      <c r="B30" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>326</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>327</v>
+      </c>
+      <c r="B32" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>328</v>
+      </c>
+      <c r="B33" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>329</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>330</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>331</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>332</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>333</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>334</v>
+      </c>
+      <c r="B39" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>335</v>
+      </c>
+      <c r="B40" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>336</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>337</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>338</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>339</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>340</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>341</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>342</v>
+      </c>
+      <c r="B47" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>343</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>344</v>
+      </c>
+      <c r="B49" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>345</v>
+      </c>
+      <c r="B50" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>346</v>
+      </c>
+      <c r="B51" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>347</v>
+      </c>
+      <c r="B52" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>348</v>
+      </c>
+      <c r="B53" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>349</v>
+      </c>
+      <c r="B54" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>350</v>
+      </c>
+      <c r="B55" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>351</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>352</v>
+      </c>
+      <c r="B57" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>353</v>
+      </c>
+      <c r="B58" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>354</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>355</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>356</v>
+      </c>
+      <c r="B61" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>357</v>
+      </c>
+      <c r="B62" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>358</v>
+      </c>
+      <c r="B63" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>359</v>
+      </c>
+      <c r="B64" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>360</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>361</v>
+      </c>
+      <c r="B66" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>362</v>
+      </c>
+      <c r="B67" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>363</v>
+      </c>
+      <c r="B68" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>364</v>
+      </c>
+      <c r="B69" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>365</v>
+      </c>
+      <c r="B70" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>366</v>
+      </c>
+      <c r="B71" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>367</v>
+      </c>
+      <c r="B72" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>368</v>
+      </c>
+      <c r="B73" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>369</v>
+      </c>
+      <c r="B74" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>370</v>
+      </c>
+      <c r="B75" s="3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1761,12 +2834,12 @@
       <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
@@ -1774,7 +2847,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1782,7 +2855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1790,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1798,7 +2871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1806,7 +2879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1814,7 +2887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1822,7 +2895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1830,7 +2903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1838,7 +2911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>45</v>
       </c>
@@ -1846,7 +2919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1854,7 +2927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>47</v>
       </c>
@@ -1862,7 +2935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1870,7 +2943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1878,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -1886,7 +2959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>51</v>
       </c>
@@ -1894,7 +2967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>52</v>
       </c>
@@ -1902,7 +2975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>289</v>
       </c>
@@ -1910,7 +2983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1918,7 +2991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1926,7 +2999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1934,7 +3007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>56</v>
       </c>
@@ -1942,7 +3015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>57</v>
       </c>
@@ -1950,7 +3023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>276</v>
       </c>
@@ -1958,7 +3031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>277</v>
       </c>
@@ -1966,7 +3039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>278</v>
       </c>
@@ -1974,7 +3047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1982,7 +3055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>59</v>
       </c>
@@ -1990,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>60</v>
       </c>
@@ -1998,7 +3071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>61</v>
       </c>
@@ -2006,7 +3079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>62</v>
       </c>
@@ -2014,7 +3087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -2022,7 +3095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
@@ -2030,7 +3103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>65</v>
       </c>
@@ -2038,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -2046,7 +3119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>67</v>
       </c>
@@ -2054,7 +3127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>68</v>
       </c>
@@ -2062,7 +3135,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>69</v>
       </c>
@@ -2070,7 +3143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>70</v>
       </c>
@@ -2078,7 +3151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>230</v>
       </c>
@@ -2086,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>231</v>
       </c>
@@ -2094,7 +3167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>232</v>
       </c>
@@ -2102,7 +3175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>233</v>
       </c>
@@ -2110,7 +3183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>234</v>
       </c>
@@ -2118,7 +3191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>235</v>
       </c>
@@ -2126,7 +3199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>236</v>
       </c>
@@ -2134,7 +3207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>237</v>
       </c>
@@ -2142,7 +3215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>238</v>
       </c>
@@ -2150,7 +3223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>239</v>
       </c>
@@ -2158,7 +3231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>240</v>
       </c>
@@ -2166,7 +3239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>282</v>
       </c>
@@ -2174,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>283</v>
       </c>
@@ -2182,7 +3255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>284</v>
       </c>
@@ -2190,7 +3263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>285</v>
       </c>
@@ -2198,7 +3271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>286</v>
       </c>
@@ -2206,7 +3279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>71</v>
       </c>
@@ -2214,7 +3287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>72</v>
       </c>
@@ -2222,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>73</v>
       </c>
@@ -2230,7 +3303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -2238,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -2246,7 +3319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>76</v>
       </c>
@@ -2254,7 +3327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>77</v>
       </c>
@@ -2262,7 +3335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>78</v>
       </c>
@@ -2270,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -2278,7 +3351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>80</v>
       </c>
@@ -2286,7 +3359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -2294,7 +3367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>82</v>
       </c>
@@ -2302,7 +3375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>83</v>
       </c>
@@ -2310,7 +3383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -2318,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -2326,7 +3399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>86</v>
       </c>
@@ -2334,7 +3407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>87</v>
       </c>
@@ -2342,7 +3415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>266</v>
       </c>
@@ -2350,7 +3423,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>267</v>
       </c>
@@ -2358,7 +3431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>268</v>
       </c>
@@ -2366,7 +3439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>269</v>
       </c>
@@ -2374,7 +3447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>270</v>
       </c>
@@ -2382,7 +3455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>271</v>
       </c>
@@ -2390,7 +3463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>272</v>
       </c>
@@ -2398,7 +3471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>273</v>
       </c>
@@ -2406,7 +3479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>274</v>
       </c>
@@ -2414,7 +3487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>88</v>
       </c>
@@ -2422,7 +3495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>89</v>
       </c>
@@ -2430,7 +3503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -2438,7 +3511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>91</v>
       </c>
@@ -2446,7 +3519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>92</v>
       </c>
@@ -2454,7 +3527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>93</v>
       </c>
@@ -2462,7 +3535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>247</v>
       </c>
@@ -2470,7 +3543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -2478,7 +3551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>97</v>
       </c>
@@ -2486,7 +3559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>95</v>
       </c>
@@ -2494,7 +3567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>96</v>
       </c>
@@ -2502,7 +3575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>248</v>
       </c>
@@ -2510,7 +3583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>98</v>
       </c>
@@ -2518,7 +3591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>263</v>
       </c>
@@ -2526,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>264</v>
       </c>
@@ -2534,7 +3607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>99</v>
       </c>
@@ -2542,7 +3615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>249</v>
       </c>
@@ -2550,7 +3623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -2558,7 +3631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>250</v>
       </c>
@@ -2566,7 +3639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>251</v>
       </c>
@@ -2574,7 +3647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>252</v>
       </c>
@@ -2582,7 +3655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>253</v>
       </c>
@@ -2590,7 +3663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>254</v>
       </c>
@@ -2598,7 +3671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>255</v>
       </c>
@@ -2606,7 +3679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>256</v>
       </c>
@@ -2614,7 +3687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>257</v>
       </c>
@@ -2622,7 +3695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>258</v>
       </c>
@@ -2630,7 +3703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>259</v>
       </c>
@@ -2638,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>260</v>
       </c>
@@ -2646,7 +3719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>261</v>
       </c>
@@ -2654,7 +3727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="2" t="s">
         <v>101</v>
       </c>
@@ -2662,7 +3735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="2" t="s">
         <v>102</v>
       </c>
@@ -2670,7 +3743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="2" t="s">
         <v>103</v>
       </c>
@@ -2678,7 +3751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="2" t="s">
         <v>104</v>
       </c>
@@ -2686,7 +3759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="2" t="s">
         <v>105</v>
       </c>
@@ -2694,7 +3767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="2" t="s">
         <v>106</v>
       </c>
@@ -2702,7 +3775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="2" t="s">
         <v>107</v>
       </c>
@@ -2710,7 +3783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
         <v>108</v>
       </c>
@@ -2718,7 +3791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="2" t="s">
         <v>109</v>
       </c>
@@ -2726,7 +3799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="2" t="s">
         <v>110</v>
       </c>
@@ -2734,7 +3807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>241</v>
       </c>
@@ -2742,7 +3815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>111</v>
       </c>
@@ -2750,7 +3823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>112</v>
       </c>
@@ -2758,7 +3831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>113</v>
       </c>
@@ -2766,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>242</v>
       </c>
@@ -2774,7 +3847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>114</v>
       </c>
@@ -2782,7 +3855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>115</v>
       </c>
@@ -2790,7 +3863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>243</v>
       </c>
@@ -2798,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>244</v>
       </c>
@@ -2806,7 +3879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>245</v>
       </c>
@@ -2814,7 +3887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>290</v>
       </c>
@@ -2822,7 +3895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>246</v>
       </c>
@@ -2830,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>226</v>
       </c>
@@ -2838,7 +3911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>229</v>
       </c>
@@ -2846,7 +3919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>116</v>
       </c>
@@ -2854,7 +3927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>292</v>
       </c>
@@ -2862,7 +3935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="2" t="s">
         <v>117</v>
       </c>
@@ -2870,7 +3943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>118</v>
       </c>
@@ -2878,7 +3951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>275</v>
       </c>
@@ -2886,7 +3959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>119</v>
       </c>
@@ -2894,7 +3967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="2" t="s">
         <v>120</v>
       </c>
@@ -2902,7 +3975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>121</v>
       </c>
@@ -2910,7 +3983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>227</v>
       </c>
@@ -2918,7 +3991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>122</v>
       </c>
@@ -2926,7 +3999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>123</v>
       </c>
@@ -2934,7 +4007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>228</v>
       </c>
@@ -2942,7 +4015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>124</v>
       </c>
@@ -2950,7 +4023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>125</v>
       </c>
@@ -2958,7 +4031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>126</v>
       </c>
@@ -2966,7 +4039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
         <v>127</v>
       </c>
@@ -2974,7 +4047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>128</v>
       </c>
@@ -2982,7 +4055,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>129</v>
       </c>
@@ -2990,7 +4063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>130</v>
       </c>
@@ -3021,12 +4094,12 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>168</v>
       </c>
@@ -3034,7 +4107,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>171</v>
       </c>
@@ -3042,7 +4115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>172</v>
       </c>
@@ -3050,7 +4123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -3058,7 +4131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>170</v>
       </c>
@@ -3066,7 +4139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>174</v>
       </c>
@@ -3074,7 +4147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>279</v>
       </c>
@@ -3082,7 +4155,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>281</v>
       </c>
@@ -3090,7 +4163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>280</v>
       </c>
@@ -3098,7 +4171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>169</v>
       </c>
@@ -3124,12 +4197,12 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>136</v>
       </c>
@@ -3137,7 +4210,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>160</v>
       </c>
@@ -3145,7 +4218,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>137</v>
       </c>
@@ -3153,7 +4226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -3161,7 +4234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -3169,7 +4242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -3177,7 +4250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -3185,7 +4258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -3193,7 +4266,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -3201,7 +4274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -3209,7 +4282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>142</v>
       </c>
@@ -3217,7 +4290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>150</v>
       </c>
@@ -3225,7 +4298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>141</v>
       </c>
@@ -3233,7 +4306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>265</v>
       </c>
@@ -3241,7 +4314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -3249,7 +4322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>262</v>
       </c>
@@ -3257,7 +4330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>164</v>
       </c>
@@ -3265,7 +4338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>153</v>
       </c>
@@ -3273,7 +4346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>151</v>
       </c>
@@ -3281,7 +4354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>152</v>
       </c>
@@ -3289,7 +4362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>287</v>
       </c>
@@ -3297,7 +4370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>288</v>
       </c>
@@ -3305,7 +4378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>157</v>
       </c>
@@ -3313,7 +4386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>159</v>
       </c>
@@ -3321,7 +4394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>148</v>
       </c>
@@ -3329,7 +4402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -3337,7 +4410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>158</v>
       </c>
@@ -3345,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>146</v>
       </c>
@@ -3353,7 +4426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>147</v>
       </c>
@@ -3361,7 +4434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>143</v>
       </c>
@@ -3369,7 +4442,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -3377,7 +4450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>145</v>
       </c>
@@ -3385,7 +4458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>155</v>
       </c>
@@ -3393,7 +4466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>155</v>
       </c>
@@ -3401,7 +4474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>291</v>
       </c>
@@ -3433,9 +4506,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>166</v>
       </c>
@@ -3443,7 +4516,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3451,7 +4524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3459,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3467,7 +4540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3475,7 +4548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3483,7 +4556,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3504,9 +4577,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>131</v>
       </c>
@@ -3514,7 +4587,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -3535,9 +4608,9 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>206</v>
       </c>
@@ -3545,7 +4618,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -3553,7 +4626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -3561,7 +4634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>178</v>
       </c>
@@ -3569,7 +4642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>179</v>
       </c>
@@ -3577,7 +4650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>180</v>
       </c>
@@ -3585,7 +4658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -3593,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>182</v>
       </c>
@@ -3601,7 +4674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>183</v>
       </c>
@@ -3609,7 +4682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>184</v>
       </c>
@@ -3617,7 +4690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>185</v>
       </c>
@@ -3625,7 +4698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>186</v>
       </c>
@@ -3633,7 +4706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>187</v>
       </c>
@@ -3641,7 +4714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>188</v>
       </c>
@@ -3649,7 +4722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>189</v>
       </c>
@@ -3657,7 +4730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>190</v>
       </c>
@@ -3665,7 +4738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>191</v>
       </c>
@@ -3673,7 +4746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>192</v>
       </c>
@@ -3681,7 +4754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>193</v>
       </c>
@@ -3698,13 +4771,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D5B3E0-498C-4AB7-BB30-7BCE295E19AC}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>205</v>
       </c>
@@ -3712,7 +4785,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>145</v>
       </c>
@@ -3720,7 +4793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>195</v>
       </c>
@@ -3728,7 +4801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>196</v>
       </c>
@@ -3736,7 +4809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>197</v>
       </c>
@@ -3744,7 +4817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>198</v>
       </c>
@@ -3752,7 +4825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>199</v>
       </c>
@@ -3760,7 +4833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>200</v>
       </c>
@@ -3768,7 +4841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>201</v>
       </c>
@@ -3776,7 +4849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>293</v>
       </c>
@@ -3797,9 +4870,9 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>204</v>
       </c>
@@ -3808,7 +4881,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2015</v>
       </c>
@@ -3816,7 +4889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2018</v>
       </c>
@@ -3824,7 +4897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2019</v>
       </c>
@@ -3832,7 +4905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2020</v>
       </c>
@@ -3840,7 +4913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -3848,7 +4921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -3856,7 +4929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -3864,7 +4937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2035</v>
       </c>
@@ -3872,7 +4945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2040</v>
       </c>
@@ -3880,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2045</v>
       </c>
@@ -3888,7 +4961,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2050</v>
       </c>
@@ -3896,7 +4969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2055</v>
       </c>
@@ -3904,7 +4977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2060</v>
       </c>

</xml_diff>